<commit_message>
starting to make purchases
</commit_message>
<xml_diff>
--- a/Production Planning/Production Planning.xlsx
+++ b/Production Planning/Production Planning.xlsx
@@ -4,34 +4,100 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Kickstarter Backer Count" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>$5 Thank you tier</t>
+  </si>
+  <si>
+    <t># of single
+clock backers</t>
+  </si>
+  <si>
+    <t>Early bird</t>
+  </si>
+  <si>
+    <t># of 2 clock backers</t>
+  </si>
+  <si>
+    <t>Regular $80</t>
+  </si>
+  <si>
+    <t>Two $159</t>
+  </si>
+  <si>
+    <t>Bulk Pack</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Total backers</t>
+  </si>
+  <si>
+    <t>Total Clocks</t>
+  </si>
+  <si>
+    <t>Actual Total Clocks</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Source Code Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Source Code Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -39,14 +105,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4146,138 +4230,138 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{9B53DD3D-F808-44CE-9400-DA35574FDA64}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" srcOrd="0" destOrd="0" parTransId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" sibTransId="{07CEFD30-6CFE-42E4-98CA-E47AFB6BB496}"/>
+    <dgm:cxn modelId="{D0C05DB1-E9AB-4E19-A8B8-637582681FA7}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{9362CB1F-15CC-4695-A870-B772FD72C8CC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{35E95C22-5E57-4231-9853-5BEF299ABD17}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" srcOrd="1" destOrd="0" parTransId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" sibTransId="{B80C44C3-7397-4BF2-A5DC-149244F61606}"/>
+    <dgm:cxn modelId="{04F72DDC-F61B-4786-B8E2-C41933CB2548}" type="presOf" srcId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" destId="{DF4CFA4A-9655-423E-BA9B-E97F7E042E15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{693A26A1-C966-4851-847F-FFCB7C69EFED}" type="presOf" srcId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" destId="{001089A2-9D3A-4B07-B5A2-E4A950A70A4B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CB72B9FF-64C5-4EA8-8106-C97705B03F53}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F2E83ED8-89A8-4994-8635-839B45715E66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C0155D02-15CB-4D10-A30E-67BFEDE13B83}" type="presOf" srcId="{BBB0F776-4554-493F-B21B-A368FA081884}" destId="{A1A1D899-7D04-49DB-9638-0AF55271E5B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BFD98051-47E4-4064-8617-215BAAE374D5}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{8B36FB09-B2AC-44F8-8F68-BE3888A0785F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7609D238-DE81-4F77-9ACB-8B9DFB43507E}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{ADD10C73-D834-4826-9754-A662C8A7E1FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{9926E8C4-11F1-4E57-8044-FA5A496F185E}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{1A2471ED-36A3-4744-9252-0E8F112223BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{983A77F7-69A6-4159-BEA3-8E0D04F4F713}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{7A03834A-A5F9-4FCF-B9B2-87650B576057}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{372E8A1E-C6E3-4637-92AA-58327BCF9C77}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B0746E47-F226-44C6-B536-D93BA85D5222}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{10F0B04D-6888-4FCF-BD8C-EB22E2BFB6EC}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{1F9A465B-2E7B-46B7-B156-012247D9FA9F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3F17C7F7-8A6E-4104-A18B-C1F8CFE7B1FA}" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" srcOrd="0" destOrd="0" parTransId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" sibTransId="{CADC4826-8984-4539-AF80-75768C983DAA}"/>
+    <dgm:cxn modelId="{E84FA001-7EDF-48D2-9BAD-7846B9FC8F20}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" srcOrd="0" destOrd="0" parTransId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" sibTransId="{3FBCBB0E-0731-4489-94AE-8BE75C8F628E}"/>
+    <dgm:cxn modelId="{E78FF662-314D-4D2D-84AB-A0BC58445FD4}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{906CFF80-8B0C-487E-8CE3-28B7CBE86B4B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5FDCA98A-1EC1-40C6-B503-EFB8A30C359A}" type="presOf" srcId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" destId="{0FC6D450-676E-4D67-AA08-5B0CF3E5AD3F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{8838431D-022D-4CCB-B56A-2B66BCDFF72C}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{78A08CF4-A659-46B7-A9CC-0C0438B9EB76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{63538616-1835-4FEB-8468-07356898D4B1}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" srcOrd="3" destOrd="0" parTransId="{21A3E433-3652-4686-B76B-CC35D311316A}" sibTransId="{28726268-BD5C-459D-A572-1342735178A8}"/>
+    <dgm:cxn modelId="{56DCF919-95F2-43CE-A1A3-CD48733A5601}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{E87EAE8A-6AEE-42F9-89D6-97AAC447F7F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9D477A73-90BA-4DFE-A7DB-63A491C9DF35}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" srcOrd="3" destOrd="0" parTransId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" sibTransId="{34C0D155-3918-433C-BD33-D4C7F3FF17B4}"/>
+    <dgm:cxn modelId="{1FF5C458-8348-4663-A257-D0C043E80854}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F6A40F5F-458E-46AC-8805-B3B47A74763F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{756C2BEC-3D3C-4382-B325-0DABD1F3DAF3}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" srcOrd="1" destOrd="0" parTransId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" sibTransId="{2A07CC88-744A-44EC-B0CC-CE24D8EFAE44}"/>
+    <dgm:cxn modelId="{580913A0-525A-4B44-B2FB-ADF82A980B51}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{B44048FB-FF46-4440-A04E-4D04E7A269DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7D5CDD5B-29EB-4B2B-8739-95D47C3F0FFA}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{C15AAE4C-4DCF-4B8D-8ED5-048AED20A2EA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E1C5F49D-7239-4EE5-8B0B-F6C8B52CD3DB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7EEDFEBA-89F9-455A-A21C-AE43DD8F2CB2}" type="presOf" srcId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" destId="{84762FF3-3F2C-409D-8C10-B0BC51085F37}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D80B63F5-D359-49B9-A49B-7ECF173D0351}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{3B170B0A-5CFE-4B48-8852-4B9BABF27377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5C31F55A-1EEC-443A-93B4-A2C4877D01D0}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{F2F22B34-EF56-4B93-8AE8-5CF39DB57AEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E0DE46DD-9F39-436A-B8F2-9959665BB989}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{6B1C35DD-3AAC-42F6-B575-AA5B770C5A88}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3D003AD7-9879-4413-9641-281F91A7322E}" type="presOf" srcId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" destId="{BC6D8F65-8D8A-4F44-A01D-A8CF55D1CCC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C823D9E6-2DEB-42C1-AF36-407405ED345F}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{0FC862D5-A8A5-4AA8-9ED4-6BE56788C7B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{796ADD97-175F-4C77-BCF6-9D630B695237}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" srcOrd="2" destOrd="0" parTransId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" sibTransId="{E90672A0-8D35-4C57-A098-707DC3A2633D}"/>
+    <dgm:cxn modelId="{CF3C6953-3C83-4E86-9462-0FD19D00C5E2}" type="presOf" srcId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" destId="{13CF6856-B59C-4292-ACC1-C9F9AEF2F240}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{AA5A3826-1016-4988-8BC5-BDCAB4010A2D}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" srcOrd="2" destOrd="0" parTransId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" sibTransId="{D62C1C4D-C034-4380-A8E3-C9B3175021C0}"/>
+    <dgm:cxn modelId="{38540A88-23DF-47C1-96FD-0E208B715EC5}" type="presOf" srcId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" destId="{4A0B8463-E60C-423F-80DC-0F37E67616B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C6C5B24C-F894-4AB8-8785-CE0FED446306}" type="presOf" srcId="{9017723E-9271-414F-97DD-42C6B68B95A5}" destId="{48F7A5C4-7657-4360-9C34-527C051DCADE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{61AC905E-18D9-45C7-AD41-05AA7D6957BC}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{7ADC2ACF-7CCE-4EDE-B698-8EF3D9E0DA94}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F5A24763-C72A-4450-A1F2-EE86CB98065C}" type="presOf" srcId="{21A3E433-3652-4686-B76B-CC35D311316A}" destId="{6F9E1F6F-E2FF-43BB-BECD-38365E7EC4E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{524220DD-557B-4AD7-B3A1-F0B75CA2F78B}" type="presOf" srcId="{94045EE5-521F-4058-B71D-61C3F9B61754}" destId="{383198C9-E9B1-4D15-B310-46BF8A1F45E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{182A552B-0968-48EF-92DC-7313BD555D2F}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{BBD1FB81-7467-4262-B91A-385D5BBCD502}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2F4C2A0D-943D-44BD-8877-CCC3BC0A5A4C}" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" srcOrd="0" destOrd="0" parTransId="{60925050-7C95-4474-807E-9FCCE6A3D0EE}" sibTransId="{DE52A88C-7199-40CB-ABEE-8AEAC1198F02}"/>
+    <dgm:cxn modelId="{98557AF7-DE82-4940-9419-216C8471C670}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FADF29D8-DCE3-42EC-868B-6E3678942948}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B63B5EFB-F838-4F48-A2B4-577DC312D528}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" srcOrd="0" destOrd="0" parTransId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" sibTransId="{FAD51D7D-047F-4498-BDAE-D5C0736263AD}"/>
+    <dgm:cxn modelId="{019CBBEB-7020-4136-A585-98DDD5FB4576}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{82458DB8-1422-4E5B-B162-76C0E86E009E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{23E1DB96-0EAB-47C7-AB8F-51EC88D2F047}" type="presOf" srcId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" destId="{DA539E27-FAC3-43D8-B720-C6B60C7F83D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{573E182D-647E-4FAE-B5A2-732E510393EA}" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" srcOrd="0" destOrd="0" parTransId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" sibTransId="{6F537722-6A7E-46BE-9FF1-4F54D9BAB5EF}"/>
+    <dgm:cxn modelId="{58CFD2E9-2A26-4A32-A1A7-29F4EDBC0A4E}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{01B84209-B4EE-4290-8B4C-72A429770547}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{09E0065A-04CD-49A7-BFF4-BB9A32C83FD9}" type="presOf" srcId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" destId="{8CC6DBE7-25F1-45E0-811F-58BFB4E6FBF9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{580913A0-525A-4B44-B2FB-ADF82A980B51}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{B44048FB-FF46-4440-A04E-4D04E7A269DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DFDF7D99-8F0C-49CB-B56D-284155AB9437}" type="presOf" srcId="{C258E371-6010-423A-B89E-97F39B6E2061}" destId="{0B1CBF2B-551A-40C7-B11C-E62ADF473FFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{35E95C22-5E57-4231-9853-5BEF299ABD17}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" srcOrd="1" destOrd="0" parTransId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" sibTransId="{B80C44C3-7397-4BF2-A5DC-149244F61606}"/>
-    <dgm:cxn modelId="{FA6F9ACA-BB6A-4731-9A4B-D5D23818E8D3}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" srcOrd="5" destOrd="0" parTransId="{623569C3-553D-47FC-917D-DD7627C010D4}" sibTransId="{246DAF3F-2D1D-4A7A-A18D-7CC64A61220B}"/>
-    <dgm:cxn modelId="{372E8A1E-C6E3-4637-92AA-58327BCF9C77}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B0746E47-F226-44C6-B536-D93BA85D5222}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{24736A80-AD67-4EE9-8F41-59367F394EF9}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{9C6F0D09-7654-49E6-BEE9-F5798519A1C7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{980F6E64-2D07-4ACB-AB41-88F91366616B}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{A1413320-E1DA-4727-8163-71C9FBE3DAA6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CB72B9FF-64C5-4EA8-8106-C97705B03F53}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F2E83ED8-89A8-4994-8635-839B45715E66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{58CFD2E9-2A26-4A32-A1A7-29F4EDBC0A4E}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{01B84209-B4EE-4290-8B4C-72A429770547}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1C4FF281-C9D4-47E5-A2D9-21D4FA56AA3D}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{D4124EAE-C9A4-44D7-8696-129097016723}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5D0ED62E-4705-4174-ABF3-044523A91C3F}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{CBF4E0AE-D8D2-4311-82F7-B8881C50572D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{61575136-175D-4FEF-BE80-70AC48BEF140}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{308C6037-FADA-4F2B-8429-2A008A44D9F2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{ECA2396E-0B8D-4627-BE94-D3842C316098}" type="presOf" srcId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" destId="{695642E2-B91F-4EE3-9EFF-1DFC56010147}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E1C5F49D-7239-4EE5-8B0B-F6C8B52CD3DB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CF3C6953-3C83-4E86-9462-0FD19D00C5E2}" type="presOf" srcId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" destId="{13CF6856-B59C-4292-ACC1-C9F9AEF2F240}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{98DBC49F-0FE8-49D1-A8E0-5BF18B6B56C6}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{019924A5-E93F-429E-913D-69BF8664489C}" srcOrd="0" destOrd="0" parTransId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" sibTransId="{B0E33302-3849-41D5-B325-A7A44C8028D5}"/>
-    <dgm:cxn modelId="{3CF0914D-8D34-4B67-83FA-23FAE4D5E70B}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{65FE7A1F-0558-481B-B958-A369D0BC2A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{4852368D-7AEA-49C1-886B-CFF58430821B}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" srcOrd="3" destOrd="0" parTransId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" sibTransId="{7E81F9C3-E4FA-4D27-8D73-380C37F4FA1A}"/>
-    <dgm:cxn modelId="{17AD505C-44DB-4307-A72F-1B5B07721D5A}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{54476BD3-5D72-4211-8A5F-213D3719457A}" srcOrd="1" destOrd="0" parTransId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" sibTransId="{37B6B00B-0731-4ED2-ABCA-2078374C26AB}"/>
-    <dgm:cxn modelId="{3F17C7F7-8A6E-4104-A18B-C1F8CFE7B1FA}" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" srcOrd="0" destOrd="0" parTransId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" sibTransId="{CADC4826-8984-4539-AF80-75768C983DAA}"/>
-    <dgm:cxn modelId="{EBD95D13-3837-406F-AF56-F1881EF797AA}" type="presOf" srcId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" destId="{144EFE5B-2652-4ADF-B7F7-8617B26DD151}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{182A552B-0968-48EF-92DC-7313BD555D2F}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{BBD1FB81-7467-4262-B91A-385D5BBCD502}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CDE8BC82-BFE5-4C51-9CF4-3237D037F4C7}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{49D6A224-676A-4B84-9205-AE4869E06BA1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{29FAD393-1AB5-4A16-8C30-205421DF1AF3}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" srcOrd="1" destOrd="0" parTransId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" sibTransId="{C25FB3F9-7E05-4DB8-BD9E-B451284794DB}"/>
-    <dgm:cxn modelId="{48B1619E-E55E-4A50-9BC2-C3DF86363710}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{D57AF638-81DE-43EB-84E2-A59C7AAADE15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{89EC6FE0-FD6B-4D2F-9491-444D5C6DDE5B}" type="presOf" srcId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" destId="{F31A2C04-E633-44C2-802F-28970E0F32FD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A2CFE446-F7AF-4625-9038-66F953BC2E23}" type="presOf" srcId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" destId="{5D8738F3-1038-4DB7-90C8-BC0BCD90DD29}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E9B02B10-502A-4259-90D4-55EFAEE3D886}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{3D6067FF-2AC1-434B-8C23-95B06FAAB7DF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C0155D02-15CB-4D10-A30E-67BFEDE13B83}" type="presOf" srcId="{BBB0F776-4554-493F-B21B-A368FA081884}" destId="{A1A1D899-7D04-49DB-9638-0AF55271E5B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2F4C2A0D-943D-44BD-8877-CCC3BC0A5A4C}" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" srcOrd="0" destOrd="0" parTransId="{60925050-7C95-4474-807E-9FCCE6A3D0EE}" sibTransId="{DE52A88C-7199-40CB-ABEE-8AEAC1198F02}"/>
-    <dgm:cxn modelId="{04F72DDC-F61B-4786-B8E2-C41933CB2548}" type="presOf" srcId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" destId="{DF4CFA4A-9655-423E-BA9B-E97F7E042E15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{79922E2F-2A52-48DE-9C7B-2E49DA66BAA6}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{CDA58B6C-10C1-4268-A158-A858D216A50B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B63B5EFB-F838-4F48-A2B4-577DC312D528}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" srcOrd="0" destOrd="0" parTransId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" sibTransId="{FAD51D7D-047F-4498-BDAE-D5C0736263AD}"/>
-    <dgm:cxn modelId="{98557AF7-DE82-4940-9419-216C8471C670}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FADF29D8-DCE3-42EC-868B-6E3678942948}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{791EB8E4-2C29-49B9-ACE9-4353F631F682}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" srcOrd="6" destOrd="0" parTransId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" sibTransId="{52EA894C-DC02-4F39-85C1-504899E0ED5C}"/>
-    <dgm:cxn modelId="{0A8B4B5C-489D-4674-B2EF-A8DE5D07769B}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" srcOrd="0" destOrd="0" parTransId="{94045EE5-521F-4058-B71D-61C3F9B61754}" sibTransId="{F03AD7E4-A782-4A9F-99F7-5327187C6D4B}"/>
-    <dgm:cxn modelId="{524220DD-557B-4AD7-B3A1-F0B75CA2F78B}" type="presOf" srcId="{94045EE5-521F-4058-B71D-61C3F9B61754}" destId="{383198C9-E9B1-4D15-B310-46BF8A1F45E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D4EF41BA-3402-4E9D-A60D-C999F57A0E84}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{95EC4EE2-724C-474F-A9E1-B85274F03474}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FDDD8B81-44D2-4EEF-BDD8-C4318390FBCD}" type="presOf" srcId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" destId="{90615ECA-3150-4DCA-B2C2-DB8382651959}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{258F77C6-606A-4A4C-AEC5-A513CB7AFD3F}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{7367E153-CE6E-45B1-8878-0762ECA2DD83}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9FBC12D3-EC0F-4FFE-B35C-B96A516268B3}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{398568D2-83C7-4580-90B1-59B85FA66394}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A8C0414D-BED6-42D6-8DFF-34CF71ED14E0}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" srcOrd="2" destOrd="0" parTransId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" sibTransId="{67E78DAB-94A4-4E9D-98CC-77C1C6804395}"/>
-    <dgm:cxn modelId="{CD1EF373-5611-4DA6-8FBA-00DD32FC09C4}" type="presOf" srcId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" destId="{AAB0485D-A3EC-4102-81CB-07D8924ADBF4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9D477A73-90BA-4DFE-A7DB-63A491C9DF35}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" srcOrd="3" destOrd="0" parTransId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" sibTransId="{34C0D155-3918-433C-BD33-D4C7F3FF17B4}"/>
-    <dgm:cxn modelId="{B7BED5F3-F8C6-4E35-A050-825A623A2466}" type="presOf" srcId="{623569C3-553D-47FC-917D-DD7627C010D4}" destId="{4A8D1159-9965-48F1-A22C-6FC96723A10A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3222FCC2-7732-41BC-9872-E843E8E156D5}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{D1ED424D-39D3-4398-AFE5-AA3426E34553}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{8CB6F1DA-9CD0-4FE5-8973-7040367FF0D6}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{2CAE613B-01AD-404A-B46B-B5DC3F4158E2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{23E1DB96-0EAB-47C7-AB8F-51EC88D2F047}" type="presOf" srcId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" destId="{DA539E27-FAC3-43D8-B720-C6B60C7F83D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{56DCF919-95F2-43CE-A1A3-CD48733A5601}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{E87EAE8A-6AEE-42F9-89D6-97AAC447F7F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{EE06ED72-436B-4261-85D9-5B0C5C947861}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{1DF726E4-1965-4D1B-B481-C845850FBD91}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{693A26A1-C966-4851-847F-FFCB7C69EFED}" type="presOf" srcId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" destId="{001089A2-9D3A-4B07-B5A2-E4A950A70A4B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FF4EBA5C-6BF9-4FF6-A464-6F57BD5A8005}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{43424605-3AA8-40DF-8879-85A13A7043A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D0C05DB1-E9AB-4E19-A8B8-637582681FA7}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{9362CB1F-15CC-4695-A870-B772FD72C8CC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{10F0B04D-6888-4FCF-BD8C-EB22E2BFB6EC}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{1F9A465B-2E7B-46B7-B156-012247D9FA9F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{BDA0D26B-B83B-49E6-B768-2EA20803F58D}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" srcOrd="1" destOrd="0" parTransId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" sibTransId="{C5BEA234-398E-4E73-A1DA-697FAA886784}"/>
-    <dgm:cxn modelId="{30E66259-DDD1-4524-BB9A-CD51F25581B7}" type="presOf" srcId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" destId="{9FA01DDC-66B0-409A-8BDE-2ACDFA7EA0A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{169CC2D5-06A5-4676-B3E1-57E444CD68DF}" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" srcOrd="0" destOrd="0" parTransId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" sibTransId="{68CE1292-8B6F-4793-B5AD-2C8C6F8E2A4C}"/>
-    <dgm:cxn modelId="{550FC2DC-30EA-4F6B-88A7-14D4D62B6D08}" type="presOf" srcId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" destId="{40DFF878-6852-49C1-B90F-9D5F087C41E0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{01DFE12C-24E7-492D-90D0-00C2CF934409}" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{0D7D100F-92B5-45B5-9725-E3A708939227}" srcOrd="1" destOrd="0" parTransId="{8A19F7E9-2BC0-4D99-ABE0-959A3B609E1F}" sibTransId="{380CE9FA-62B1-4DE2-A53B-AD49F2297CFA}"/>
     <dgm:cxn modelId="{4E5BA1A2-CAB7-4D2B-850D-C1BD85B5AC02}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{63808121-E830-4E2A-B990-90E7F621E30F}" srcOrd="2" destOrd="0" parTransId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" sibTransId="{0B660145-ABA6-4795-9573-394A26CE26B5}"/>
+    <dgm:cxn modelId="{FF4EBA5C-6BF9-4FF6-A464-6F57BD5A8005}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{43424605-3AA8-40DF-8879-85A13A7043A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{791EB8E4-2C29-49B9-ACE9-4353F631F682}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" srcOrd="6" destOrd="0" parTransId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" sibTransId="{52EA894C-DC02-4F39-85C1-504899E0ED5C}"/>
+    <dgm:cxn modelId="{8CB6F1DA-9CD0-4FE5-8973-7040367FF0D6}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{2CAE613B-01AD-404A-B46B-B5DC3F4158E2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FDDD8B81-44D2-4EEF-BDD8-C4318390FBCD}" type="presOf" srcId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" destId="{90615ECA-3150-4DCA-B2C2-DB8382651959}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CD1EF373-5611-4DA6-8FBA-00DD32FC09C4}" type="presOf" srcId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" destId="{AAB0485D-A3EC-4102-81CB-07D8924ADBF4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CF1D7D51-67B3-4504-B651-9017E70040F5}" type="presOf" srcId="{8A19F7E9-2BC0-4D99-ABE0-959A3B609E1F}" destId="{92F80147-D6CE-494A-B3BF-F945F8928DBB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{89EC6FE0-FD6B-4D2F-9491-444D5C6DDE5B}" type="presOf" srcId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" destId="{F31A2C04-E633-44C2-802F-28970E0F32FD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{829F191D-B2D5-4B9E-8363-9C4759B32AC5}" type="presOf" srcId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" destId="{767CE880-7FEE-4F49-BC75-EEADD920D80C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CDE8BC82-BFE5-4C51-9CF4-3237D037F4C7}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{49D6A224-676A-4B84-9205-AE4869E06BA1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2484F9C7-26A2-49A1-BC42-413A7983B278}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{B7ACCDD8-83B3-40B2-9381-9FF766A19F2E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7BE10628-CF64-476D-BB2C-641D6E8DC54D}" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" srcOrd="0" destOrd="0" parTransId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" sibTransId="{23383EFD-FF7C-4A80-8967-E663AC937494}"/>
+    <dgm:cxn modelId="{2962B927-1A21-4C72-B520-A6CCD31698F6}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{ACD37203-AD9C-4240-AEB3-595C59E85038}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{169CC2D5-06A5-4676-B3E1-57E444CD68DF}" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" srcOrd="0" destOrd="0" parTransId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" sibTransId="{68CE1292-8B6F-4793-B5AD-2C8C6F8E2A4C}"/>
+    <dgm:cxn modelId="{FDA0BC06-C109-4213-A9FD-AB9A246DA1F4}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{C8B363C0-C0D5-41D3-865A-D32D640BB9C2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{59A4C806-2DC3-43D7-BD98-65332CF12A61}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" srcOrd="0" destOrd="0" parTransId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" sibTransId="{504954EE-ED7B-492D-A310-649ECE5BE26E}"/>
+    <dgm:cxn modelId="{5D0ED62E-4705-4174-ABF3-044523A91C3F}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{CBF4E0AE-D8D2-4311-82F7-B8881C50572D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A7A24DFE-09AF-45FE-99EB-EE36C7772AF1}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{9400333F-4396-4E18-9C39-78B617E7CE6E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CAB7C766-CF1B-4C8A-A5D4-F3AB6C7ABE05}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{1724DB36-8A28-458A-BF68-E63DA8F29DB2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{4735EF70-45BC-42FF-B63E-7CC9819AC9B0}" type="presOf" srcId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" destId="{09F4703B-18C0-422F-86B1-DFD11C06CB69}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3CF0914D-8D34-4B67-83FA-23FAE4D5E70B}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{65FE7A1F-0558-481B-B958-A369D0BC2A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DA103A88-0446-4BDD-8087-1C5821541D25}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{4B293DCB-D5C3-471C-92C9-34A400F5E89E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DFDF7D99-8F0C-49CB-B56D-284155AB9437}" type="presOf" srcId="{C258E371-6010-423A-B89E-97F39B6E2061}" destId="{0B1CBF2B-551A-40C7-B11C-E62ADF473FFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3222FCC2-7732-41BC-9872-E843E8E156D5}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{D1ED424D-39D3-4398-AFE5-AA3426E34553}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9B53DD3D-F808-44CE-9400-DA35574FDA64}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" srcOrd="0" destOrd="0" parTransId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" sibTransId="{07CEFD30-6CFE-42E4-98CA-E47AFB6BB496}"/>
+    <dgm:cxn modelId="{56FA2085-EADC-4A6E-8AA4-BE27C0E4B20D}" type="presOf" srcId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" destId="{6B91EE95-DB69-4714-969D-213267DBB176}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B7BED5F3-F8C6-4E35-A050-825A623A2466}" type="presOf" srcId="{623569C3-553D-47FC-917D-DD7627C010D4}" destId="{4A8D1159-9965-48F1-A22C-6FC96723A10A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{22167890-A4E5-4F19-B6D4-C7F0A9D6F243}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{26ED289C-3010-4451-ADDD-F478A5C75B6B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E9D8D529-E009-4058-8BE5-B856001724FF}" type="presOf" srcId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" destId="{E13783EC-3280-454C-9EDC-7AD64A0482B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FBC579E8-AF02-4F0D-932E-0C08AEA2481B}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{173AA79E-2FF2-42D4-B70B-D125E9A80658}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0A8B4B5C-489D-4674-B2EF-A8DE5D07769B}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" srcOrd="0" destOrd="0" parTransId="{94045EE5-521F-4058-B71D-61C3F9B61754}" sibTransId="{F03AD7E4-A782-4A9F-99F7-5327187C6D4B}"/>
+    <dgm:cxn modelId="{F8823ED8-8E0C-492B-BE83-EE8C541E88F4}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{3B55DA41-6AB2-41A4-A264-27032A092EF8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DF3E8A34-5921-4655-A3D3-F6D91E7F34C0}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3635EF60-F64E-4EE3-B729-086102104583}" srcOrd="0" destOrd="0" parTransId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" sibTransId="{A2ECA061-8B56-4FB6-B1DA-2A310FA48213}"/>
+    <dgm:cxn modelId="{9EA12656-6C66-47B0-9920-C69C30E2F618}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{03FB1A03-C635-4199-880D-D1975DFAC8B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A9D4B4A0-1484-479A-93D6-399996E6A1B6}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{B978A0BD-405C-4642-9A48-ACCBC26BAC87}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{01F81704-8185-4782-B291-C9FB2BA43C0B}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{D0AE8A71-F0F1-4838-A3CA-B0981E423524}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{ADAD5ADC-43E6-4343-8682-1862D42E3DA9}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{7137C75B-9DFD-4BD4-820F-1EF47882DDDC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{AB3F6E07-EDB4-42D9-B306-B85C11273364}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{32ABA577-60BD-4197-902B-F86B9051CAE1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{44477E50-1F68-4929-8394-94CD5C1E0479}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{8686384B-DEFF-498F-B380-F68C33BD97BB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{29FAD393-1AB5-4A16-8C30-205421DF1AF3}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" srcOrd="1" destOrd="0" parTransId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" sibTransId="{C25FB3F9-7E05-4DB8-BD9E-B451284794DB}"/>
+    <dgm:cxn modelId="{A2AD75FE-A88F-4066-9437-801D13701F0D}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{EB689344-4045-416E-B23F-1ED7CCF7A250}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A8C0414D-BED6-42D6-8DFF-34CF71ED14E0}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" srcOrd="2" destOrd="0" parTransId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" sibTransId="{67E78DAB-94A4-4E9D-98CC-77C1C6804395}"/>
+    <dgm:cxn modelId="{A2CFE446-F7AF-4625-9038-66F953BC2E23}" type="presOf" srcId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" destId="{5D8738F3-1038-4DB7-90C8-BC0BCD90DD29}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{502D1E8E-ABC4-4B81-B07D-71307B16B28A}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{92B83617-ED82-479A-81AB-48E59441279A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{4852368D-7AEA-49C1-886B-CFF58430821B}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" srcOrd="3" destOrd="0" parTransId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" sibTransId="{7E81F9C3-E4FA-4D27-8D73-380C37F4FA1A}"/>
+    <dgm:cxn modelId="{A73AD1F8-380E-4C75-A752-6AD7EAD4AF16}" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" srcOrd="0" destOrd="0" parTransId="{BBB0F776-4554-493F-B21B-A368FA081884}" sibTransId="{717A4BC5-2FD2-4D7A-912F-D3F9F37D4AC4}"/>
+    <dgm:cxn modelId="{ECA2396E-0B8D-4627-BE94-D3842C316098}" type="presOf" srcId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" destId="{695642E2-B91F-4EE3-9EFF-1DFC56010147}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{30E66259-DDD1-4524-BB9A-CD51F25581B7}" type="presOf" srcId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" destId="{9FA01DDC-66B0-409A-8BDE-2ACDFA7EA0A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9768AB10-23AB-47C4-874B-92CBB49B9235}" type="presOf" srcId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" destId="{426E8D05-299B-4227-83F5-A25FDC0795CE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1E25BA0B-AA21-4599-8237-94C90FA1318F}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" srcOrd="1" destOrd="0" parTransId="{9017723E-9271-414F-97DD-42C6B68B95A5}" sibTransId="{F3B1A03B-8586-468D-AB33-0AF66DB1B805}"/>
+    <dgm:cxn modelId="{E9B02B10-502A-4259-90D4-55EFAEE3D886}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{3D6067FF-2AC1-434B-8C23-95B06FAAB7DF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{258F77C6-606A-4A4C-AEC5-A513CB7AFD3F}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{7367E153-CE6E-45B1-8878-0762ECA2DD83}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{61575136-175D-4FEF-BE80-70AC48BEF140}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{308C6037-FADA-4F2B-8429-2A008A44D9F2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{33D79453-008A-4D1E-90E8-873B3083C39C}" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" srcOrd="0" destOrd="0" parTransId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" sibTransId="{5B17D466-83AB-4A1E-8366-95071FB481AC}"/>
+    <dgm:cxn modelId="{1C4FF281-C9D4-47E5-A2D9-21D4FA56AA3D}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{D4124EAE-C9A4-44D7-8696-129097016723}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A96ED176-342B-4CCE-B6C9-05774EA877F2}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{5E40320B-C876-487B-B530-CDD6B4496081}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9031E8AF-6292-4901-914C-42E38AF62562}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{E74FDBBE-303A-48BD-9525-0327D908A1D2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{24736A80-AD67-4EE9-8F41-59367F394EF9}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{9C6F0D09-7654-49E6-BEE9-F5798519A1C7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{79922E2F-2A52-48DE-9C7B-2E49DA66BAA6}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{CDA58B6C-10C1-4268-A158-A858D216A50B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{98DBC49F-0FE8-49D1-A8E0-5BF18B6B56C6}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{019924A5-E93F-429E-913D-69BF8664489C}" srcOrd="0" destOrd="0" parTransId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" sibTransId="{B0E33302-3849-41D5-B325-A7A44C8028D5}"/>
     <dgm:cxn modelId="{9B24C8EB-FEC3-4361-8F6A-C004F72B6CA5}" type="presOf" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{CA7202EA-FC9B-469A-818E-C42165B0D395}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7BE10628-CF64-476D-BB2C-641D6E8DC54D}" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" srcOrd="0" destOrd="0" parTransId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" sibTransId="{23383EFD-FF7C-4A80-8967-E663AC937494}"/>
-    <dgm:cxn modelId="{FDA0BC06-C109-4213-A9FD-AB9A246DA1F4}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{C8B363C0-C0D5-41D3-865A-D32D640BB9C2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5FDCA98A-1EC1-40C6-B503-EFB8A30C359A}" type="presOf" srcId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" destId="{0FC6D450-676E-4D67-AA08-5B0CF3E5AD3F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7609D238-DE81-4F77-9ACB-8B9DFB43507E}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{ADD10C73-D834-4826-9754-A662C8A7E1FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5C31F55A-1EEC-443A-93B4-A2C4877D01D0}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{F2F22B34-EF56-4B93-8AE8-5CF39DB57AEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FBC579E8-AF02-4F0D-932E-0C08AEA2481B}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{173AA79E-2FF2-42D4-B70B-D125E9A80658}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{24B53B70-2C73-4B1D-90C0-D891A86675A0}" type="presOf" srcId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" destId="{A7886049-F4A6-4B3E-BF2E-DBE90C832EAD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2C948CFD-02CA-4B5C-B3F4-F0D8A68C91AE}" type="presOf" srcId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" destId="{A2733577-E6F8-490F-BDFB-91F1859D51F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0027E26B-B643-4445-B18E-D376D30650B3}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" srcOrd="2" destOrd="0" parTransId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" sibTransId="{BCE61832-DA7C-4F87-BB86-D5835E40DAB1}"/>
+    <dgm:cxn modelId="{EBD95D13-3837-406F-AF56-F1881EF797AA}" type="presOf" srcId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" destId="{144EFE5B-2652-4ADF-B7F7-8617B26DD151}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B008CD50-423B-4D30-8552-0611AF438E08}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FECE3617-7B45-4E8D-A2CB-852EA32699A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0FA33ECD-AB07-4C39-88F5-784DEA5392D4}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{64252D07-EE7B-49E9-8905-77D83680C8CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{4AE052C3-7ADC-475C-B793-20DC671F3A9A}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" srcOrd="1" destOrd="0" parTransId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" sibTransId="{476294FA-2A8D-4342-AA14-A29092D8CBE3}"/>
+    <dgm:cxn modelId="{BDA0D26B-B83B-49E6-B768-2EA20803F58D}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" srcOrd="1" destOrd="0" parTransId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" sibTransId="{C5BEA234-398E-4E73-A1DA-697FAA886784}"/>
+    <dgm:cxn modelId="{D4EF41BA-3402-4E9D-A60D-C999F57A0E84}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{95EC4EE2-724C-474F-A9E1-B85274F03474}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9FBC12D3-EC0F-4FFE-B35C-B96A516268B3}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{398568D2-83C7-4580-90B1-59B85FA66394}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{40DA832C-FAE3-4AC1-BFAF-6393F8A574E2}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{EA0793E8-65F4-4383-82A2-4170B37B05B1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9C2291B3-6308-483B-8E34-9D7E5B8D8FDB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{FB94CB6F-F13A-4A1C-BC5B-21260572171F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{F6471420-45D0-4883-AA73-794106838C93}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{B4FB48FE-BE0C-42D7-AE54-FF62EFDAA971}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{829F191D-B2D5-4B9E-8363-9C4759B32AC5}" type="presOf" srcId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" destId="{767CE880-7FEE-4F49-BC75-EEADD920D80C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{F5A24763-C72A-4450-A1F2-EE86CB98065C}" type="presOf" srcId="{21A3E433-3652-4686-B76B-CC35D311316A}" destId="{6F9E1F6F-E2FF-43BB-BECD-38365E7EC4E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{61AC905E-18D9-45C7-AD41-05AA7D6957BC}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{7ADC2ACF-7CCE-4EDE-B698-8EF3D9E0DA94}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9C2291B3-6308-483B-8E34-9D7E5B8D8FDB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{FB94CB6F-F13A-4A1C-BC5B-21260572171F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{F8823ED8-8E0C-492B-BE83-EE8C541E88F4}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{3B55DA41-6AB2-41A4-A264-27032A092EF8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AB3F6E07-EDB4-42D9-B306-B85C11273364}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{32ABA577-60BD-4197-902B-F86B9051CAE1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{38540A88-23DF-47C1-96FD-0E208B715EC5}" type="presOf" srcId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" destId="{4A0B8463-E60C-423F-80DC-0F37E67616B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7D5CDD5B-29EB-4B2B-8739-95D47C3F0FFA}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{C15AAE4C-4DCF-4B8D-8ED5-048AED20A2EA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{502D1E8E-ABC4-4B81-B07D-71307B16B28A}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{92B83617-ED82-479A-81AB-48E59441279A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{17AD505C-44DB-4307-A72F-1B5B07721D5A}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{54476BD3-5D72-4211-8A5F-213D3719457A}" srcOrd="1" destOrd="0" parTransId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" sibTransId="{37B6B00B-0731-4ED2-ABCA-2078374C26AB}"/>
+    <dgm:cxn modelId="{FA6F9ACA-BB6A-4731-9A4B-D5D23818E8D3}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" srcOrd="5" destOrd="0" parTransId="{623569C3-553D-47FC-917D-DD7627C010D4}" sibTransId="{246DAF3F-2D1D-4A7A-A18D-7CC64A61220B}"/>
+    <dgm:cxn modelId="{FC50FAD2-3727-4FE2-87C4-B5ADDCB292B0}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" srcOrd="4" destOrd="0" parTransId="{C258E371-6010-423A-B89E-97F39B6E2061}" sibTransId="{D11DF62A-C599-40F2-883D-4E7E458CF1F8}"/>
+    <dgm:cxn modelId="{550FC2DC-30EA-4F6B-88A7-14D4D62B6D08}" type="presOf" srcId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" destId="{40DFF878-6852-49C1-B90F-9D5F087C41E0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{E8B7A71D-511C-48F7-BE47-FAE4F15A1514}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{43450866-70F5-4361-BB5A-08446B43F641}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{24B53B70-2C73-4B1D-90C0-D891A86675A0}" type="presOf" srcId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" destId="{A7886049-F4A6-4B3E-BF2E-DBE90C832EAD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C6C5B24C-F894-4AB8-8785-CE0FED446306}" type="presOf" srcId="{9017723E-9271-414F-97DD-42C6B68B95A5}" destId="{48F7A5C4-7657-4360-9C34-527C051DCADE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0FA33ECD-AB07-4C39-88F5-784DEA5392D4}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{64252D07-EE7B-49E9-8905-77D83680C8CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DF3E8A34-5921-4655-A3D3-F6D91E7F34C0}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3635EF60-F64E-4EE3-B729-086102104583}" srcOrd="0" destOrd="0" parTransId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" sibTransId="{A2ECA061-8B56-4FB6-B1DA-2A310FA48213}"/>
-    <dgm:cxn modelId="{22167890-A4E5-4F19-B6D4-C7F0A9D6F243}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{26ED289C-3010-4451-ADDD-F478A5C75B6B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E84FA001-7EDF-48D2-9BAD-7846B9FC8F20}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" srcOrd="0" destOrd="0" parTransId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" sibTransId="{3FBCBB0E-0731-4489-94AE-8BE75C8F628E}"/>
-    <dgm:cxn modelId="{756C2BEC-3D3C-4382-B325-0DABD1F3DAF3}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" srcOrd="1" destOrd="0" parTransId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" sibTransId="{2A07CC88-744A-44EC-B0CC-CE24D8EFAE44}"/>
-    <dgm:cxn modelId="{0027E26B-B643-4445-B18E-D376D30650B3}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" srcOrd="2" destOrd="0" parTransId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" sibTransId="{BCE61832-DA7C-4F87-BB86-D5835E40DAB1}"/>
-    <dgm:cxn modelId="{C823D9E6-2DEB-42C1-AF36-407405ED345F}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{0FC862D5-A8A5-4AA8-9ED4-6BE56788C7B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{8838431D-022D-4CCB-B56A-2B66BCDFF72C}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{78A08CF4-A659-46B7-A9CC-0C0438B9EB76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3D003AD7-9879-4413-9641-281F91A7322E}" type="presOf" srcId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" destId="{BC6D8F65-8D8A-4F44-A01D-A8CF55D1CCC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{019CBBEB-7020-4136-A585-98DDD5FB4576}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{82458DB8-1422-4E5B-B162-76C0E86E009E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B008CD50-423B-4D30-8552-0611AF438E08}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FECE3617-7B45-4E8D-A2CB-852EA32699A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{01F81704-8185-4782-B291-C9FB2BA43C0B}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{D0AE8A71-F0F1-4838-A3CA-B0981E423524}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A7A24DFE-09AF-45FE-99EB-EE36C7772AF1}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{9400333F-4396-4E18-9C39-78B617E7CE6E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9031E8AF-6292-4901-914C-42E38AF62562}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{E74FDBBE-303A-48BD-9525-0327D908A1D2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AA5A3826-1016-4988-8BC5-BDCAB4010A2D}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" srcOrd="2" destOrd="0" parTransId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" sibTransId="{D62C1C4D-C034-4380-A8E3-C9B3175021C0}"/>
-    <dgm:cxn modelId="{4735EF70-45BC-42FF-B63E-7CC9819AC9B0}" type="presOf" srcId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" destId="{09F4703B-18C0-422F-86B1-DFD11C06CB69}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D80B63F5-D359-49B9-A49B-7ECF173D0351}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{3B170B0A-5CFE-4B48-8852-4B9BABF27377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E0DE46DD-9F39-436A-B8F2-9959665BB989}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{6B1C35DD-3AAC-42F6-B575-AA5B770C5A88}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2C948CFD-02CA-4B5C-B3F4-F0D8A68C91AE}" type="presOf" srcId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" destId="{A2733577-E6F8-490F-BDFB-91F1859D51F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2484F9C7-26A2-49A1-BC42-413A7983B278}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{B7ACCDD8-83B3-40B2-9381-9FF766A19F2E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1E25BA0B-AA21-4599-8237-94C90FA1318F}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" srcOrd="1" destOrd="0" parTransId="{9017723E-9271-414F-97DD-42C6B68B95A5}" sibTransId="{F3B1A03B-8586-468D-AB33-0AF66DB1B805}"/>
-    <dgm:cxn modelId="{FC50FAD2-3727-4FE2-87C4-B5ADDCB292B0}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" srcOrd="4" destOrd="0" parTransId="{C258E371-6010-423A-B89E-97F39B6E2061}" sibTransId="{D11DF62A-C599-40F2-883D-4E7E458CF1F8}"/>
-    <dgm:cxn modelId="{796ADD97-175F-4C77-BCF6-9D630B695237}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" srcOrd="2" destOrd="0" parTransId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" sibTransId="{E90672A0-8D35-4C57-A098-707DC3A2633D}"/>
-    <dgm:cxn modelId="{9EA12656-6C66-47B0-9920-C69C30E2F618}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{03FB1A03-C635-4199-880D-D1975DFAC8B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E78FF662-314D-4D2D-84AB-A0BC58445FD4}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{906CFF80-8B0C-487E-8CE3-28B7CBE86B4B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1FF5C458-8348-4663-A257-D0C043E80854}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F6A40F5F-458E-46AC-8805-B3B47A74763F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2962B927-1A21-4C72-B520-A6CCD31698F6}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{ACD37203-AD9C-4240-AEB3-595C59E85038}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{40DA832C-FAE3-4AC1-BFAF-6393F8A574E2}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{EA0793E8-65F4-4383-82A2-4170B37B05B1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{44477E50-1F68-4929-8394-94CD5C1E0479}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{8686384B-DEFF-498F-B380-F68C33BD97BB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{63538616-1835-4FEB-8468-07356898D4B1}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" srcOrd="3" destOrd="0" parTransId="{21A3E433-3652-4686-B76B-CC35D311316A}" sibTransId="{28726268-BD5C-459D-A572-1342735178A8}"/>
-    <dgm:cxn modelId="{BFD98051-47E4-4064-8617-215BAAE374D5}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{8B36FB09-B2AC-44F8-8F68-BE3888A0785F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{56FA2085-EADC-4A6E-8AA4-BE27C0E4B20D}" type="presOf" srcId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" destId="{6B91EE95-DB69-4714-969D-213267DBB176}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E9D8D529-E009-4058-8BE5-B856001724FF}" type="presOf" srcId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" destId="{E13783EC-3280-454C-9EDC-7AD64A0482B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{59A4C806-2DC3-43D7-BD98-65332CF12A61}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" srcOrd="0" destOrd="0" parTransId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" sibTransId="{504954EE-ED7B-492D-A310-649ECE5BE26E}"/>
-    <dgm:cxn modelId="{4AE052C3-7ADC-475C-B793-20DC671F3A9A}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" srcOrd="1" destOrd="0" parTransId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" sibTransId="{476294FA-2A8D-4342-AA14-A29092D8CBE3}"/>
-    <dgm:cxn modelId="{CAB7C766-CF1B-4C8A-A5D4-F3AB6C7ABE05}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{1724DB36-8A28-458A-BF68-E63DA8F29DB2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{983A77F7-69A6-4159-BEA3-8E0D04F4F713}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{7A03834A-A5F9-4FCF-B9B2-87650B576057}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{EE06ED72-436B-4261-85D9-5B0C5C947861}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{1DF726E4-1965-4D1B-B481-C845850FBD91}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{C8106DA2-C15B-4E1D-BE48-04DF11A0A4B4}" type="presOf" srcId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" destId="{F7C0520F-A4DD-4BA0-8CE1-746C13CB31D3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9768AB10-23AB-47C4-874B-92CBB49B9235}" type="presOf" srcId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" destId="{426E8D05-299B-4227-83F5-A25FDC0795CE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DA103A88-0446-4BDD-8087-1C5821541D25}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{4B293DCB-D5C3-471C-92C9-34A400F5E89E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{ADAD5ADC-43E6-4343-8682-1862D42E3DA9}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{7137C75B-9DFD-4BD4-820F-1EF47882DDDC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7EEDFEBA-89F9-455A-A21C-AE43DD8F2CB2}" type="presOf" srcId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" destId="{84762FF3-3F2C-409D-8C10-B0BC51085F37}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A2AD75FE-A88F-4066-9437-801D13701F0D}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{EB689344-4045-416E-B23F-1ED7CCF7A250}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A9D4B4A0-1484-479A-93D6-399996E6A1B6}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{B978A0BD-405C-4642-9A48-ACCBC26BAC87}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{33D79453-008A-4D1E-90E8-873B3083C39C}" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" srcOrd="0" destOrd="0" parTransId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" sibTransId="{5B17D466-83AB-4A1E-8366-95071FB481AC}"/>
-    <dgm:cxn modelId="{573E182D-647E-4FAE-B5A2-732E510393EA}" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" srcOrd="0" destOrd="0" parTransId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" sibTransId="{6F537722-6A7E-46BE-9FF1-4F54D9BAB5EF}"/>
-    <dgm:cxn modelId="{A96ED176-342B-4CCE-B6C9-05774EA877F2}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{5E40320B-C876-487B-B530-CDD6B4496081}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CF1D7D51-67B3-4504-B651-9017E70040F5}" type="presOf" srcId="{8A19F7E9-2BC0-4D99-ABE0-959A3B609E1F}" destId="{92F80147-D6CE-494A-B3BF-F945F8928DBB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A73AD1F8-380E-4C75-A752-6AD7EAD4AF16}" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" srcOrd="0" destOrd="0" parTransId="{BBB0F776-4554-493F-B21B-A368FA081884}" sibTransId="{717A4BC5-2FD2-4D7A-912F-D3F9F37D4AC4}"/>
+    <dgm:cxn modelId="{48B1619E-E55E-4A50-9BC2-C3DF86363710}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{D57AF638-81DE-43EB-84E2-A59C7AAADE15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{980F6E64-2D07-4ACB-AB41-88F91366616B}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{A1413320-E1DA-4727-8163-71C9FBE3DAA6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{A2A34727-EEDD-4F7A-B70A-FADD1FED13E9}" type="presParOf" srcId="{CA7202EA-FC9B-469A-818E-C42165B0D395}" destId="{83E344F5-8732-4AE4-B4CF-AA653D5BC4D1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{3F8D4B7B-4C1F-43E7-8217-64B98642208E}" type="presParOf" srcId="{83E344F5-8732-4AE4-B4CF-AA653D5BC4D1}" destId="{26D0847B-F0A1-4E26-8E2B-16FCF79D4617}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{5EFA0D23-DF22-4371-BCF6-EC7E58F4AD0E}" type="presParOf" srcId="{26D0847B-F0A1-4E26-8E2B-16FCF79D4617}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -11471,7 +11555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -11480,4 +11564,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>99-11</f>
+        <v>88</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C4:C9)</f>
+        <v>325</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:E11" si="0">SUM(D4:D9)</f>
+        <v>46</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <f>C11*1</f>
+        <v>325</v>
+      </c>
+      <c r="D12" s="3">
+        <f>D11*2</f>
+        <v>92</v>
+      </c>
+      <c r="E12" s="3">
+        <f>E11*5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
+        <f>SUM(C12:E12)</f>
+        <v>427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B10:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="47.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
production planning and purchases
</commit_message>
<xml_diff>
--- a/Production Planning/Production Planning.xlsx
+++ b/Production Planning/Production Planning.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Kickstarter Backer Count" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -56,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,7 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -127,7 +126,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
@@ -4230,138 +4228,138 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{9B53DD3D-F808-44CE-9400-DA35574FDA64}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" srcOrd="0" destOrd="0" parTransId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" sibTransId="{07CEFD30-6CFE-42E4-98CA-E47AFB6BB496}"/>
+    <dgm:cxn modelId="{9926E8C4-11F1-4E57-8044-FA5A496F185E}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{1A2471ED-36A3-4744-9252-0E8F112223BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{09E0065A-04CD-49A7-BFF4-BB9A32C83FD9}" type="presOf" srcId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" destId="{8CC6DBE7-25F1-45E0-811F-58BFB4E6FBF9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{580913A0-525A-4B44-B2FB-ADF82A980B51}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{B44048FB-FF46-4440-A04E-4D04E7A269DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DFDF7D99-8F0C-49CB-B56D-284155AB9437}" type="presOf" srcId="{C258E371-6010-423A-B89E-97F39B6E2061}" destId="{0B1CBF2B-551A-40C7-B11C-E62ADF473FFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{35E95C22-5E57-4231-9853-5BEF299ABD17}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" srcOrd="1" destOrd="0" parTransId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" sibTransId="{B80C44C3-7397-4BF2-A5DC-149244F61606}"/>
+    <dgm:cxn modelId="{FA6F9ACA-BB6A-4731-9A4B-D5D23818E8D3}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" srcOrd="5" destOrd="0" parTransId="{623569C3-553D-47FC-917D-DD7627C010D4}" sibTransId="{246DAF3F-2D1D-4A7A-A18D-7CC64A61220B}"/>
+    <dgm:cxn modelId="{372E8A1E-C6E3-4637-92AA-58327BCF9C77}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B0746E47-F226-44C6-B536-D93BA85D5222}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{24736A80-AD67-4EE9-8F41-59367F394EF9}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{9C6F0D09-7654-49E6-BEE9-F5798519A1C7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{980F6E64-2D07-4ACB-AB41-88F91366616B}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{A1413320-E1DA-4727-8163-71C9FBE3DAA6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CB72B9FF-64C5-4EA8-8106-C97705B03F53}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F2E83ED8-89A8-4994-8635-839B45715E66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{58CFD2E9-2A26-4A32-A1A7-29F4EDBC0A4E}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{01B84209-B4EE-4290-8B4C-72A429770547}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1C4FF281-C9D4-47E5-A2D9-21D4FA56AA3D}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{D4124EAE-C9A4-44D7-8696-129097016723}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5D0ED62E-4705-4174-ABF3-044523A91C3F}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{CBF4E0AE-D8D2-4311-82F7-B8881C50572D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{61575136-175D-4FEF-BE80-70AC48BEF140}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{308C6037-FADA-4F2B-8429-2A008A44D9F2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{ECA2396E-0B8D-4627-BE94-D3842C316098}" type="presOf" srcId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" destId="{695642E2-B91F-4EE3-9EFF-1DFC56010147}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E1C5F49D-7239-4EE5-8B0B-F6C8B52CD3DB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CF3C6953-3C83-4E86-9462-0FD19D00C5E2}" type="presOf" srcId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" destId="{13CF6856-B59C-4292-ACC1-C9F9AEF2F240}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{98DBC49F-0FE8-49D1-A8E0-5BF18B6B56C6}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{019924A5-E93F-429E-913D-69BF8664489C}" srcOrd="0" destOrd="0" parTransId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" sibTransId="{B0E33302-3849-41D5-B325-A7A44C8028D5}"/>
+    <dgm:cxn modelId="{3CF0914D-8D34-4B67-83FA-23FAE4D5E70B}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{65FE7A1F-0558-481B-B958-A369D0BC2A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{4852368D-7AEA-49C1-886B-CFF58430821B}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" srcOrd="3" destOrd="0" parTransId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" sibTransId="{7E81F9C3-E4FA-4D27-8D73-380C37F4FA1A}"/>
+    <dgm:cxn modelId="{17AD505C-44DB-4307-A72F-1B5B07721D5A}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{54476BD3-5D72-4211-8A5F-213D3719457A}" srcOrd="1" destOrd="0" parTransId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" sibTransId="{37B6B00B-0731-4ED2-ABCA-2078374C26AB}"/>
+    <dgm:cxn modelId="{3F17C7F7-8A6E-4104-A18B-C1F8CFE7B1FA}" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" srcOrd="0" destOrd="0" parTransId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" sibTransId="{CADC4826-8984-4539-AF80-75768C983DAA}"/>
+    <dgm:cxn modelId="{EBD95D13-3837-406F-AF56-F1881EF797AA}" type="presOf" srcId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" destId="{144EFE5B-2652-4ADF-B7F7-8617B26DD151}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{182A552B-0968-48EF-92DC-7313BD555D2F}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{BBD1FB81-7467-4262-B91A-385D5BBCD502}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CDE8BC82-BFE5-4C51-9CF4-3237D037F4C7}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{49D6A224-676A-4B84-9205-AE4869E06BA1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{29FAD393-1AB5-4A16-8C30-205421DF1AF3}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" srcOrd="1" destOrd="0" parTransId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" sibTransId="{C25FB3F9-7E05-4DB8-BD9E-B451284794DB}"/>
+    <dgm:cxn modelId="{48B1619E-E55E-4A50-9BC2-C3DF86363710}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{D57AF638-81DE-43EB-84E2-A59C7AAADE15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{89EC6FE0-FD6B-4D2F-9491-444D5C6DDE5B}" type="presOf" srcId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" destId="{F31A2C04-E633-44C2-802F-28970E0F32FD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A2CFE446-F7AF-4625-9038-66F953BC2E23}" type="presOf" srcId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" destId="{5D8738F3-1038-4DB7-90C8-BC0BCD90DD29}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E9B02B10-502A-4259-90D4-55EFAEE3D886}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{3D6067FF-2AC1-434B-8C23-95B06FAAB7DF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C0155D02-15CB-4D10-A30E-67BFEDE13B83}" type="presOf" srcId="{BBB0F776-4554-493F-B21B-A368FA081884}" destId="{A1A1D899-7D04-49DB-9638-0AF55271E5B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2F4C2A0D-943D-44BD-8877-CCC3BC0A5A4C}" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" srcOrd="0" destOrd="0" parTransId="{60925050-7C95-4474-807E-9FCCE6A3D0EE}" sibTransId="{DE52A88C-7199-40CB-ABEE-8AEAC1198F02}"/>
+    <dgm:cxn modelId="{04F72DDC-F61B-4786-B8E2-C41933CB2548}" type="presOf" srcId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" destId="{DF4CFA4A-9655-423E-BA9B-E97F7E042E15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{79922E2F-2A52-48DE-9C7B-2E49DA66BAA6}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{CDA58B6C-10C1-4268-A158-A858D216A50B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B63B5EFB-F838-4F48-A2B4-577DC312D528}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" srcOrd="0" destOrd="0" parTransId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" sibTransId="{FAD51D7D-047F-4498-BDAE-D5C0736263AD}"/>
+    <dgm:cxn modelId="{98557AF7-DE82-4940-9419-216C8471C670}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FADF29D8-DCE3-42EC-868B-6E3678942948}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{791EB8E4-2C29-49B9-ACE9-4353F631F682}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" srcOrd="6" destOrd="0" parTransId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" sibTransId="{52EA894C-DC02-4F39-85C1-504899E0ED5C}"/>
+    <dgm:cxn modelId="{0A8B4B5C-489D-4674-B2EF-A8DE5D07769B}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" srcOrd="0" destOrd="0" parTransId="{94045EE5-521F-4058-B71D-61C3F9B61754}" sibTransId="{F03AD7E4-A782-4A9F-99F7-5327187C6D4B}"/>
+    <dgm:cxn modelId="{524220DD-557B-4AD7-B3A1-F0B75CA2F78B}" type="presOf" srcId="{94045EE5-521F-4058-B71D-61C3F9B61754}" destId="{383198C9-E9B1-4D15-B310-46BF8A1F45E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D4EF41BA-3402-4E9D-A60D-C999F57A0E84}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{95EC4EE2-724C-474F-A9E1-B85274F03474}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FDDD8B81-44D2-4EEF-BDD8-C4318390FBCD}" type="presOf" srcId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" destId="{90615ECA-3150-4DCA-B2C2-DB8382651959}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{258F77C6-606A-4A4C-AEC5-A513CB7AFD3F}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{7367E153-CE6E-45B1-8878-0762ECA2DD83}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9FBC12D3-EC0F-4FFE-B35C-B96A516268B3}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{398568D2-83C7-4580-90B1-59B85FA66394}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A8C0414D-BED6-42D6-8DFF-34CF71ED14E0}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" srcOrd="2" destOrd="0" parTransId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" sibTransId="{67E78DAB-94A4-4E9D-98CC-77C1C6804395}"/>
+    <dgm:cxn modelId="{CD1EF373-5611-4DA6-8FBA-00DD32FC09C4}" type="presOf" srcId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" destId="{AAB0485D-A3EC-4102-81CB-07D8924ADBF4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9D477A73-90BA-4DFE-A7DB-63A491C9DF35}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" srcOrd="3" destOrd="0" parTransId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" sibTransId="{34C0D155-3918-433C-BD33-D4C7F3FF17B4}"/>
+    <dgm:cxn modelId="{B7BED5F3-F8C6-4E35-A050-825A623A2466}" type="presOf" srcId="{623569C3-553D-47FC-917D-DD7627C010D4}" destId="{4A8D1159-9965-48F1-A22C-6FC96723A10A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3222FCC2-7732-41BC-9872-E843E8E156D5}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{D1ED424D-39D3-4398-AFE5-AA3426E34553}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{8CB6F1DA-9CD0-4FE5-8973-7040367FF0D6}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{2CAE613B-01AD-404A-B46B-B5DC3F4158E2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{23E1DB96-0EAB-47C7-AB8F-51EC88D2F047}" type="presOf" srcId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" destId="{DA539E27-FAC3-43D8-B720-C6B60C7F83D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{56DCF919-95F2-43CE-A1A3-CD48733A5601}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{E87EAE8A-6AEE-42F9-89D6-97AAC447F7F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{EE06ED72-436B-4261-85D9-5B0C5C947861}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{1DF726E4-1965-4D1B-B481-C845850FBD91}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{693A26A1-C966-4851-847F-FFCB7C69EFED}" type="presOf" srcId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" destId="{001089A2-9D3A-4B07-B5A2-E4A950A70A4B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FF4EBA5C-6BF9-4FF6-A464-6F57BD5A8005}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{43424605-3AA8-40DF-8879-85A13A7043A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{D0C05DB1-E9AB-4E19-A8B8-637582681FA7}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{9362CB1F-15CC-4695-A870-B772FD72C8CC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{35E95C22-5E57-4231-9853-5BEF299ABD17}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" srcOrd="1" destOrd="0" parTransId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" sibTransId="{B80C44C3-7397-4BF2-A5DC-149244F61606}"/>
-    <dgm:cxn modelId="{04F72DDC-F61B-4786-B8E2-C41933CB2548}" type="presOf" srcId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" destId="{DF4CFA4A-9655-423E-BA9B-E97F7E042E15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{693A26A1-C966-4851-847F-FFCB7C69EFED}" type="presOf" srcId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" destId="{001089A2-9D3A-4B07-B5A2-E4A950A70A4B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CB72B9FF-64C5-4EA8-8106-C97705B03F53}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F2E83ED8-89A8-4994-8635-839B45715E66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C0155D02-15CB-4D10-A30E-67BFEDE13B83}" type="presOf" srcId="{BBB0F776-4554-493F-B21B-A368FA081884}" destId="{A1A1D899-7D04-49DB-9638-0AF55271E5B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{BFD98051-47E4-4064-8617-215BAAE374D5}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{8B36FB09-B2AC-44F8-8F68-BE3888A0785F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7609D238-DE81-4F77-9ACB-8B9DFB43507E}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{ADD10C73-D834-4826-9754-A662C8A7E1FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9926E8C4-11F1-4E57-8044-FA5A496F185E}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{1A2471ED-36A3-4744-9252-0E8F112223BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{983A77F7-69A6-4159-BEA3-8E0D04F4F713}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{7A03834A-A5F9-4FCF-B9B2-87650B576057}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{372E8A1E-C6E3-4637-92AA-58327BCF9C77}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B0746E47-F226-44C6-B536-D93BA85D5222}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{10F0B04D-6888-4FCF-BD8C-EB22E2BFB6EC}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{1F9A465B-2E7B-46B7-B156-012247D9FA9F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3F17C7F7-8A6E-4104-A18B-C1F8CFE7B1FA}" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" srcOrd="0" destOrd="0" parTransId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" sibTransId="{CADC4826-8984-4539-AF80-75768C983DAA}"/>
-    <dgm:cxn modelId="{E84FA001-7EDF-48D2-9BAD-7846B9FC8F20}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" srcOrd="0" destOrd="0" parTransId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" sibTransId="{3FBCBB0E-0731-4489-94AE-8BE75C8F628E}"/>
-    <dgm:cxn modelId="{E78FF662-314D-4D2D-84AB-A0BC58445FD4}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{906CFF80-8B0C-487E-8CE3-28B7CBE86B4B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5FDCA98A-1EC1-40C6-B503-EFB8A30C359A}" type="presOf" srcId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" destId="{0FC6D450-676E-4D67-AA08-5B0CF3E5AD3F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{8838431D-022D-4CCB-B56A-2B66BCDFF72C}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{78A08CF4-A659-46B7-A9CC-0C0438B9EB76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{63538616-1835-4FEB-8468-07356898D4B1}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" srcOrd="3" destOrd="0" parTransId="{21A3E433-3652-4686-B76B-CC35D311316A}" sibTransId="{28726268-BD5C-459D-A572-1342735178A8}"/>
-    <dgm:cxn modelId="{56DCF919-95F2-43CE-A1A3-CD48733A5601}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{E87EAE8A-6AEE-42F9-89D6-97AAC447F7F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9D477A73-90BA-4DFE-A7DB-63A491C9DF35}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" srcOrd="3" destOrd="0" parTransId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" sibTransId="{34C0D155-3918-433C-BD33-D4C7F3FF17B4}"/>
-    <dgm:cxn modelId="{1FF5C458-8348-4663-A257-D0C043E80854}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F6A40F5F-458E-46AC-8805-B3B47A74763F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{756C2BEC-3D3C-4382-B325-0DABD1F3DAF3}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" srcOrd="1" destOrd="0" parTransId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" sibTransId="{2A07CC88-744A-44EC-B0CC-CE24D8EFAE44}"/>
-    <dgm:cxn modelId="{580913A0-525A-4B44-B2FB-ADF82A980B51}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{B44048FB-FF46-4440-A04E-4D04E7A269DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7D5CDD5B-29EB-4B2B-8739-95D47C3F0FFA}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{C15AAE4C-4DCF-4B8D-8ED5-048AED20A2EA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E1C5F49D-7239-4EE5-8B0B-F6C8B52CD3DB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7EEDFEBA-89F9-455A-A21C-AE43DD8F2CB2}" type="presOf" srcId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" destId="{84762FF3-3F2C-409D-8C10-B0BC51085F37}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D80B63F5-D359-49B9-A49B-7ECF173D0351}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{3B170B0A-5CFE-4B48-8852-4B9BABF27377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5C31F55A-1EEC-443A-93B4-A2C4877D01D0}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{F2F22B34-EF56-4B93-8AE8-5CF39DB57AEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E0DE46DD-9F39-436A-B8F2-9959665BB989}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{6B1C35DD-3AAC-42F6-B575-AA5B770C5A88}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3D003AD7-9879-4413-9641-281F91A7322E}" type="presOf" srcId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" destId="{BC6D8F65-8D8A-4F44-A01D-A8CF55D1CCC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C823D9E6-2DEB-42C1-AF36-407405ED345F}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{0FC862D5-A8A5-4AA8-9ED4-6BE56788C7B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{796ADD97-175F-4C77-BCF6-9D630B695237}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" srcOrd="2" destOrd="0" parTransId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" sibTransId="{E90672A0-8D35-4C57-A098-707DC3A2633D}"/>
-    <dgm:cxn modelId="{CF3C6953-3C83-4E86-9462-0FD19D00C5E2}" type="presOf" srcId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" destId="{13CF6856-B59C-4292-ACC1-C9F9AEF2F240}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AA5A3826-1016-4988-8BC5-BDCAB4010A2D}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" srcOrd="2" destOrd="0" parTransId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" sibTransId="{D62C1C4D-C034-4380-A8E3-C9B3175021C0}"/>
-    <dgm:cxn modelId="{38540A88-23DF-47C1-96FD-0E208B715EC5}" type="presOf" srcId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" destId="{4A0B8463-E60C-423F-80DC-0F37E67616B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C6C5B24C-F894-4AB8-8785-CE0FED446306}" type="presOf" srcId="{9017723E-9271-414F-97DD-42C6B68B95A5}" destId="{48F7A5C4-7657-4360-9C34-527C051DCADE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{61AC905E-18D9-45C7-AD41-05AA7D6957BC}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{7ADC2ACF-7CCE-4EDE-B698-8EF3D9E0DA94}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{F5A24763-C72A-4450-A1F2-EE86CB98065C}" type="presOf" srcId="{21A3E433-3652-4686-B76B-CC35D311316A}" destId="{6F9E1F6F-E2FF-43BB-BECD-38365E7EC4E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{524220DD-557B-4AD7-B3A1-F0B75CA2F78B}" type="presOf" srcId="{94045EE5-521F-4058-B71D-61C3F9B61754}" destId="{383198C9-E9B1-4D15-B310-46BF8A1F45E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{182A552B-0968-48EF-92DC-7313BD555D2F}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{BBD1FB81-7467-4262-B91A-385D5BBCD502}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2F4C2A0D-943D-44BD-8877-CCC3BC0A5A4C}" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" srcOrd="0" destOrd="0" parTransId="{60925050-7C95-4474-807E-9FCCE6A3D0EE}" sibTransId="{DE52A88C-7199-40CB-ABEE-8AEAC1198F02}"/>
-    <dgm:cxn modelId="{98557AF7-DE82-4940-9419-216C8471C670}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FADF29D8-DCE3-42EC-868B-6E3678942948}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B63B5EFB-F838-4F48-A2B4-577DC312D528}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" srcOrd="0" destOrd="0" parTransId="{1190306D-AE84-41A2-B8C1-ADFB190151E6}" sibTransId="{FAD51D7D-047F-4498-BDAE-D5C0736263AD}"/>
-    <dgm:cxn modelId="{019CBBEB-7020-4136-A585-98DDD5FB4576}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{82458DB8-1422-4E5B-B162-76C0E86E009E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{23E1DB96-0EAB-47C7-AB8F-51EC88D2F047}" type="presOf" srcId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" destId="{DA539E27-FAC3-43D8-B720-C6B60C7F83D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{573E182D-647E-4FAE-B5A2-732E510393EA}" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" srcOrd="0" destOrd="0" parTransId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" sibTransId="{6F537722-6A7E-46BE-9FF1-4F54D9BAB5EF}"/>
-    <dgm:cxn modelId="{58CFD2E9-2A26-4A32-A1A7-29F4EDBC0A4E}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{01B84209-B4EE-4290-8B4C-72A429770547}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{09E0065A-04CD-49A7-BFF4-BB9A32C83FD9}" type="presOf" srcId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" destId="{8CC6DBE7-25F1-45E0-811F-58BFB4E6FBF9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BDA0D26B-B83B-49E6-B768-2EA20803F58D}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" srcOrd="1" destOrd="0" parTransId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" sibTransId="{C5BEA234-398E-4E73-A1DA-697FAA886784}"/>
+    <dgm:cxn modelId="{30E66259-DDD1-4524-BB9A-CD51F25581B7}" type="presOf" srcId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" destId="{9FA01DDC-66B0-409A-8BDE-2ACDFA7EA0A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{169CC2D5-06A5-4676-B3E1-57E444CD68DF}" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" srcOrd="0" destOrd="0" parTransId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" sibTransId="{68CE1292-8B6F-4793-B5AD-2C8C6F8E2A4C}"/>
+    <dgm:cxn modelId="{550FC2DC-30EA-4F6B-88A7-14D4D62B6D08}" type="presOf" srcId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" destId="{40DFF878-6852-49C1-B90F-9D5F087C41E0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{01DFE12C-24E7-492D-90D0-00C2CF934409}" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{0D7D100F-92B5-45B5-9725-E3A708939227}" srcOrd="1" destOrd="0" parTransId="{8A19F7E9-2BC0-4D99-ABE0-959A3B609E1F}" sibTransId="{380CE9FA-62B1-4DE2-A53B-AD49F2297CFA}"/>
     <dgm:cxn modelId="{4E5BA1A2-CAB7-4D2B-850D-C1BD85B5AC02}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{63808121-E830-4E2A-B990-90E7F621E30F}" srcOrd="2" destOrd="0" parTransId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" sibTransId="{0B660145-ABA6-4795-9573-394A26CE26B5}"/>
-    <dgm:cxn modelId="{FF4EBA5C-6BF9-4FF6-A464-6F57BD5A8005}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{43424605-3AA8-40DF-8879-85A13A7043A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{791EB8E4-2C29-49B9-ACE9-4353F631F682}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" srcOrd="6" destOrd="0" parTransId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" sibTransId="{52EA894C-DC02-4F39-85C1-504899E0ED5C}"/>
-    <dgm:cxn modelId="{8CB6F1DA-9CD0-4FE5-8973-7040367FF0D6}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{2CAE613B-01AD-404A-B46B-B5DC3F4158E2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FDDD8B81-44D2-4EEF-BDD8-C4318390FBCD}" type="presOf" srcId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" destId="{90615ECA-3150-4DCA-B2C2-DB8382651959}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CD1EF373-5611-4DA6-8FBA-00DD32FC09C4}" type="presOf" srcId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" destId="{AAB0485D-A3EC-4102-81CB-07D8924ADBF4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9B24C8EB-FEC3-4361-8F6A-C004F72B6CA5}" type="presOf" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{CA7202EA-FC9B-469A-818E-C42165B0D395}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7BE10628-CF64-476D-BB2C-641D6E8DC54D}" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" srcOrd="0" destOrd="0" parTransId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" sibTransId="{23383EFD-FF7C-4A80-8967-E663AC937494}"/>
+    <dgm:cxn modelId="{FDA0BC06-C109-4213-A9FD-AB9A246DA1F4}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{C8B363C0-C0D5-41D3-865A-D32D640BB9C2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5FDCA98A-1EC1-40C6-B503-EFB8A30C359A}" type="presOf" srcId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" destId="{0FC6D450-676E-4D67-AA08-5B0CF3E5AD3F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7609D238-DE81-4F77-9ACB-8B9DFB43507E}" type="presOf" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{ADD10C73-D834-4826-9754-A662C8A7E1FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5C31F55A-1EEC-443A-93B4-A2C4877D01D0}" type="presOf" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{F2F22B34-EF56-4B93-8AE8-5CF39DB57AEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FBC579E8-AF02-4F0D-932E-0C08AEA2481B}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{173AA79E-2FF2-42D4-B70B-D125E9A80658}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F6471420-45D0-4883-AA73-794106838C93}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{B4FB48FE-BE0C-42D7-AE54-FF62EFDAA971}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{829F191D-B2D5-4B9E-8363-9C4759B32AC5}" type="presOf" srcId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" destId="{767CE880-7FEE-4F49-BC75-EEADD920D80C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F5A24763-C72A-4450-A1F2-EE86CB98065C}" type="presOf" srcId="{21A3E433-3652-4686-B76B-CC35D311316A}" destId="{6F9E1F6F-E2FF-43BB-BECD-38365E7EC4E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{61AC905E-18D9-45C7-AD41-05AA7D6957BC}" type="presOf" srcId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" destId="{7ADC2ACF-7CCE-4EDE-B698-8EF3D9E0DA94}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9C2291B3-6308-483B-8E34-9D7E5B8D8FDB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{FB94CB6F-F13A-4A1C-BC5B-21260572171F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F8823ED8-8E0C-492B-BE83-EE8C541E88F4}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{3B55DA41-6AB2-41A4-A264-27032A092EF8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{AB3F6E07-EDB4-42D9-B306-B85C11273364}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{32ABA577-60BD-4197-902B-F86B9051CAE1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{38540A88-23DF-47C1-96FD-0E208B715EC5}" type="presOf" srcId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" destId="{4A0B8463-E60C-423F-80DC-0F37E67616B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7D5CDD5B-29EB-4B2B-8739-95D47C3F0FFA}" type="presOf" srcId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" destId="{C15AAE4C-4DCF-4B8D-8ED5-048AED20A2EA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{502D1E8E-ABC4-4B81-B07D-71307B16B28A}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{92B83617-ED82-479A-81AB-48E59441279A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E8B7A71D-511C-48F7-BE47-FAE4F15A1514}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{43450866-70F5-4361-BB5A-08446B43F641}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{24B53B70-2C73-4B1D-90C0-D891A86675A0}" type="presOf" srcId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" destId="{A7886049-F4A6-4B3E-BF2E-DBE90C832EAD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C6C5B24C-F894-4AB8-8785-CE0FED446306}" type="presOf" srcId="{9017723E-9271-414F-97DD-42C6B68B95A5}" destId="{48F7A5C4-7657-4360-9C34-527C051DCADE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0FA33ECD-AB07-4C39-88F5-784DEA5392D4}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{64252D07-EE7B-49E9-8905-77D83680C8CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DF3E8A34-5921-4655-A3D3-F6D91E7F34C0}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3635EF60-F64E-4EE3-B729-086102104583}" srcOrd="0" destOrd="0" parTransId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" sibTransId="{A2ECA061-8B56-4FB6-B1DA-2A310FA48213}"/>
+    <dgm:cxn modelId="{22167890-A4E5-4F19-B6D4-C7F0A9D6F243}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{26ED289C-3010-4451-ADDD-F478A5C75B6B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E84FA001-7EDF-48D2-9BAD-7846B9FC8F20}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" srcOrd="0" destOrd="0" parTransId="{7A4EB925-3D66-4596-B9A4-C1636F3474D1}" sibTransId="{3FBCBB0E-0731-4489-94AE-8BE75C8F628E}"/>
+    <dgm:cxn modelId="{756C2BEC-3D3C-4382-B325-0DABD1F3DAF3}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" srcOrd="1" destOrd="0" parTransId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" sibTransId="{2A07CC88-744A-44EC-B0CC-CE24D8EFAE44}"/>
+    <dgm:cxn modelId="{0027E26B-B643-4445-B18E-D376D30650B3}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" srcOrd="2" destOrd="0" parTransId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" sibTransId="{BCE61832-DA7C-4F87-BB86-D5835E40DAB1}"/>
+    <dgm:cxn modelId="{C823D9E6-2DEB-42C1-AF36-407405ED345F}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{0FC862D5-A8A5-4AA8-9ED4-6BE56788C7B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{8838431D-022D-4CCB-B56A-2B66BCDFF72C}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{78A08CF4-A659-46B7-A9CC-0C0438B9EB76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{3D003AD7-9879-4413-9641-281F91A7322E}" type="presOf" srcId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" destId="{BC6D8F65-8D8A-4F44-A01D-A8CF55D1CCC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{019CBBEB-7020-4136-A585-98DDD5FB4576}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{82458DB8-1422-4E5B-B162-76C0E86E009E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B008CD50-423B-4D30-8552-0611AF438E08}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FECE3617-7B45-4E8D-A2CB-852EA32699A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{01F81704-8185-4782-B291-C9FB2BA43C0B}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{D0AE8A71-F0F1-4838-A3CA-B0981E423524}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A7A24DFE-09AF-45FE-99EB-EE36C7772AF1}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{9400333F-4396-4E18-9C39-78B617E7CE6E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9031E8AF-6292-4901-914C-42E38AF62562}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{E74FDBBE-303A-48BD-9525-0327D908A1D2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{AA5A3826-1016-4988-8BC5-BDCAB4010A2D}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" srcOrd="2" destOrd="0" parTransId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" sibTransId="{D62C1C4D-C034-4380-A8E3-C9B3175021C0}"/>
+    <dgm:cxn modelId="{4735EF70-45BC-42FF-B63E-7CC9819AC9B0}" type="presOf" srcId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" destId="{09F4703B-18C0-422F-86B1-DFD11C06CB69}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D80B63F5-D359-49B9-A49B-7ECF173D0351}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{3B170B0A-5CFE-4B48-8852-4B9BABF27377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E0DE46DD-9F39-436A-B8F2-9959665BB989}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{6B1C35DD-3AAC-42F6-B575-AA5B770C5A88}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2C948CFD-02CA-4B5C-B3F4-F0D8A68C91AE}" type="presOf" srcId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" destId="{A2733577-E6F8-490F-BDFB-91F1859D51F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2484F9C7-26A2-49A1-BC42-413A7983B278}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{B7ACCDD8-83B3-40B2-9381-9FF766A19F2E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1E25BA0B-AA21-4599-8237-94C90FA1318F}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" srcOrd="1" destOrd="0" parTransId="{9017723E-9271-414F-97DD-42C6B68B95A5}" sibTransId="{F3B1A03B-8586-468D-AB33-0AF66DB1B805}"/>
+    <dgm:cxn modelId="{FC50FAD2-3727-4FE2-87C4-B5ADDCB292B0}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" srcOrd="4" destOrd="0" parTransId="{C258E371-6010-423A-B89E-97F39B6E2061}" sibTransId="{D11DF62A-C599-40F2-883D-4E7E458CF1F8}"/>
+    <dgm:cxn modelId="{796ADD97-175F-4C77-BCF6-9D630B695237}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" srcOrd="2" destOrd="0" parTransId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" sibTransId="{E90672A0-8D35-4C57-A098-707DC3A2633D}"/>
+    <dgm:cxn modelId="{9EA12656-6C66-47B0-9920-C69C30E2F618}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{03FB1A03-C635-4199-880D-D1975DFAC8B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E78FF662-314D-4D2D-84AB-A0BC58445FD4}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{906CFF80-8B0C-487E-8CE3-28B7CBE86B4B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1FF5C458-8348-4663-A257-D0C043E80854}" type="presOf" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{F6A40F5F-458E-46AC-8805-B3B47A74763F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2962B927-1A21-4C72-B520-A6CCD31698F6}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{ACD37203-AD9C-4240-AEB3-595C59E85038}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{40DA832C-FAE3-4AC1-BFAF-6393F8A574E2}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{EA0793E8-65F4-4383-82A2-4170B37B05B1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{44477E50-1F68-4929-8394-94CD5C1E0479}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{8686384B-DEFF-498F-B380-F68C33BD97BB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{63538616-1835-4FEB-8468-07356898D4B1}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" srcOrd="3" destOrd="0" parTransId="{21A3E433-3652-4686-B76B-CC35D311316A}" sibTransId="{28726268-BD5C-459D-A572-1342735178A8}"/>
+    <dgm:cxn modelId="{BFD98051-47E4-4064-8617-215BAAE374D5}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{8B36FB09-B2AC-44F8-8F68-BE3888A0785F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{56FA2085-EADC-4A6E-8AA4-BE27C0E4B20D}" type="presOf" srcId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" destId="{6B91EE95-DB69-4714-969D-213267DBB176}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E9D8D529-E009-4058-8BE5-B856001724FF}" type="presOf" srcId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" destId="{E13783EC-3280-454C-9EDC-7AD64A0482B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{59A4C806-2DC3-43D7-BD98-65332CF12A61}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" srcOrd="0" destOrd="0" parTransId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" sibTransId="{504954EE-ED7B-492D-A310-649ECE5BE26E}"/>
+    <dgm:cxn modelId="{4AE052C3-7ADC-475C-B793-20DC671F3A9A}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" srcOrd="1" destOrd="0" parTransId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" sibTransId="{476294FA-2A8D-4342-AA14-A29092D8CBE3}"/>
+    <dgm:cxn modelId="{CAB7C766-CF1B-4C8A-A5D4-F3AB6C7ABE05}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{1724DB36-8A28-458A-BF68-E63DA8F29DB2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{983A77F7-69A6-4159-BEA3-8E0D04F4F713}" type="presOf" srcId="{019924A5-E93F-429E-913D-69BF8664489C}" destId="{7A03834A-A5F9-4FCF-B9B2-87650B576057}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C8106DA2-C15B-4E1D-BE48-04DF11A0A4B4}" type="presOf" srcId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" destId="{F7C0520F-A4DD-4BA0-8CE1-746C13CB31D3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9768AB10-23AB-47C4-874B-92CBB49B9235}" type="presOf" srcId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" destId="{426E8D05-299B-4227-83F5-A25FDC0795CE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DA103A88-0446-4BDD-8087-1C5821541D25}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{4B293DCB-D5C3-471C-92C9-34A400F5E89E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{ADAD5ADC-43E6-4343-8682-1862D42E3DA9}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{7137C75B-9DFD-4BD4-820F-1EF47882DDDC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7EEDFEBA-89F9-455A-A21C-AE43DD8F2CB2}" type="presOf" srcId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" destId="{84762FF3-3F2C-409D-8C10-B0BC51085F37}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A2AD75FE-A88F-4066-9437-801D13701F0D}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{EB689344-4045-416E-B23F-1ED7CCF7A250}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A9D4B4A0-1484-479A-93D6-399996E6A1B6}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{B978A0BD-405C-4642-9A48-ACCBC26BAC87}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{33D79453-008A-4D1E-90E8-873B3083C39C}" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" srcOrd="0" destOrd="0" parTransId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" sibTransId="{5B17D466-83AB-4A1E-8366-95071FB481AC}"/>
+    <dgm:cxn modelId="{573E182D-647E-4FAE-B5A2-732E510393EA}" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{C93D04CB-A0E8-4015-90D9-652C191E5DA2}" srcOrd="0" destOrd="0" parTransId="{D06262AD-B99E-4BDC-B31D-3B965316A74E}" sibTransId="{6F537722-6A7E-46BE-9FF1-4F54D9BAB5EF}"/>
+    <dgm:cxn modelId="{A96ED176-342B-4CCE-B6C9-05774EA877F2}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{5E40320B-C876-487B-B530-CDD6B4496081}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{CF1D7D51-67B3-4504-B651-9017E70040F5}" type="presOf" srcId="{8A19F7E9-2BC0-4D99-ABE0-959A3B609E1F}" destId="{92F80147-D6CE-494A-B3BF-F945F8928DBB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{89EC6FE0-FD6B-4D2F-9491-444D5C6DDE5B}" type="presOf" srcId="{9FCB9D9D-D9D2-4DEE-B7BA-689E8123FFC3}" destId="{F31A2C04-E633-44C2-802F-28970E0F32FD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{829F191D-B2D5-4B9E-8363-9C4759B32AC5}" type="presOf" srcId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" destId="{767CE880-7FEE-4F49-BC75-EEADD920D80C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CDE8BC82-BFE5-4C51-9CF4-3237D037F4C7}" type="presOf" srcId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" destId="{49D6A224-676A-4B84-9205-AE4869E06BA1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2484F9C7-26A2-49A1-BC42-413A7983B278}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{B7ACCDD8-83B3-40B2-9381-9FF766A19F2E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7BE10628-CF64-476D-BB2C-641D6E8DC54D}" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" srcOrd="0" destOrd="0" parTransId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" sibTransId="{23383EFD-FF7C-4A80-8967-E663AC937494}"/>
-    <dgm:cxn modelId="{2962B927-1A21-4C72-B520-A6CCD31698F6}" type="presOf" srcId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" destId="{ACD37203-AD9C-4240-AEB3-595C59E85038}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{169CC2D5-06A5-4676-B3E1-57E444CD68DF}" srcId="{54476BD3-5D72-4211-8A5F-213D3719457A}" destId="{9E67D354-90E2-4FE9-AD10-39EFAF0D73CF}" srcOrd="0" destOrd="0" parTransId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" sibTransId="{68CE1292-8B6F-4793-B5AD-2C8C6F8E2A4C}"/>
-    <dgm:cxn modelId="{FDA0BC06-C109-4213-A9FD-AB9A246DA1F4}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{C8B363C0-C0D5-41D3-865A-D32D640BB9C2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{59A4C806-2DC3-43D7-BD98-65332CF12A61}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" srcOrd="0" destOrd="0" parTransId="{C46B43D9-2C6B-4FD2-A36D-EBB63388CEFF}" sibTransId="{504954EE-ED7B-492D-A310-649ECE5BE26E}"/>
-    <dgm:cxn modelId="{5D0ED62E-4705-4174-ABF3-044523A91C3F}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{CBF4E0AE-D8D2-4311-82F7-B8881C50572D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A7A24DFE-09AF-45FE-99EB-EE36C7772AF1}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{9400333F-4396-4E18-9C39-78B617E7CE6E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CAB7C766-CF1B-4C8A-A5D4-F3AB6C7ABE05}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{1724DB36-8A28-458A-BF68-E63DA8F29DB2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{4735EF70-45BC-42FF-B63E-7CC9819AC9B0}" type="presOf" srcId="{80AD9038-50A1-4CBD-BF09-D5213FE42327}" destId="{09F4703B-18C0-422F-86B1-DFD11C06CB69}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3CF0914D-8D34-4B67-83FA-23FAE4D5E70B}" type="presOf" srcId="{60BCFD60-18C2-4140-9C4F-DC559039811F}" destId="{65FE7A1F-0558-481B-B958-A369D0BC2A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DA103A88-0446-4BDD-8087-1C5821541D25}" type="presOf" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{4B293DCB-D5C3-471C-92C9-34A400F5E89E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DFDF7D99-8F0C-49CB-B56D-284155AB9437}" type="presOf" srcId="{C258E371-6010-423A-B89E-97F39B6E2061}" destId="{0B1CBF2B-551A-40C7-B11C-E62ADF473FFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3222FCC2-7732-41BC-9872-E843E8E156D5}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{D1ED424D-39D3-4398-AFE5-AA3426E34553}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9B53DD3D-F808-44CE-9400-DA35574FDA64}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" srcOrd="0" destOrd="0" parTransId="{65F8352B-80BD-41B5-B698-3F01F4E784B7}" sibTransId="{07CEFD30-6CFE-42E4-98CA-E47AFB6BB496}"/>
-    <dgm:cxn modelId="{56FA2085-EADC-4A6E-8AA4-BE27C0E4B20D}" type="presOf" srcId="{5866BF8D-140B-4956-9248-08D69AC4FCDD}" destId="{6B91EE95-DB69-4714-969D-213267DBB176}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B7BED5F3-F8C6-4E35-A050-825A623A2466}" type="presOf" srcId="{623569C3-553D-47FC-917D-DD7627C010D4}" destId="{4A8D1159-9965-48F1-A22C-6FC96723A10A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{22167890-A4E5-4F19-B6D4-C7F0A9D6F243}" type="presOf" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{26ED289C-3010-4451-ADDD-F478A5C75B6B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E9D8D529-E009-4058-8BE5-B856001724FF}" type="presOf" srcId="{6FE48CA7-6A45-44CD-9808-D2D2464BFD50}" destId="{E13783EC-3280-454C-9EDC-7AD64A0482B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FBC579E8-AF02-4F0D-932E-0C08AEA2481B}" type="presOf" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{173AA79E-2FF2-42D4-B70B-D125E9A80658}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0A8B4B5C-489D-4674-B2EF-A8DE5D07769B}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" srcOrd="0" destOrd="0" parTransId="{94045EE5-521F-4058-B71D-61C3F9B61754}" sibTransId="{F03AD7E4-A782-4A9F-99F7-5327187C6D4B}"/>
-    <dgm:cxn modelId="{F8823ED8-8E0C-492B-BE83-EE8C541E88F4}" type="presOf" srcId="{2AA5028E-841A-408D-8921-8B49042C1FCF}" destId="{3B55DA41-6AB2-41A4-A264-27032A092EF8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DF3E8A34-5921-4655-A3D3-F6D91E7F34C0}" srcId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" destId="{3635EF60-F64E-4EE3-B729-086102104583}" srcOrd="0" destOrd="0" parTransId="{2FC29ADB-DE29-4E9B-A909-DE75E95334B3}" sibTransId="{A2ECA061-8B56-4FB6-B1DA-2A310FA48213}"/>
-    <dgm:cxn modelId="{9EA12656-6C66-47B0-9920-C69C30E2F618}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{03FB1A03-C635-4199-880D-D1975DFAC8B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A9D4B4A0-1484-479A-93D6-399996E6A1B6}" type="presOf" srcId="{B346F646-8C49-4A12-AFAB-DD7B61F83512}" destId="{B978A0BD-405C-4642-9A48-ACCBC26BAC87}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{01F81704-8185-4782-B291-C9FB2BA43C0B}" type="presOf" srcId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" destId="{D0AE8A71-F0F1-4838-A3CA-B0981E423524}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{ADAD5ADC-43E6-4343-8682-1862D42E3DA9}" type="presOf" srcId="{391370F4-B732-4B35-B60E-8375F4CCB9AB}" destId="{7137C75B-9DFD-4BD4-820F-1EF47882DDDC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AB3F6E07-EDB4-42D9-B306-B85C11273364}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{32ABA577-60BD-4197-902B-F86B9051CAE1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{44477E50-1F68-4929-8394-94CD5C1E0479}" type="presOf" srcId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" destId="{8686384B-DEFF-498F-B380-F68C33BD97BB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{29FAD393-1AB5-4A16-8C30-205421DF1AF3}" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" srcOrd="1" destOrd="0" parTransId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" sibTransId="{C25FB3F9-7E05-4DB8-BD9E-B451284794DB}"/>
-    <dgm:cxn modelId="{A2AD75FE-A88F-4066-9437-801D13701F0D}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{EB689344-4045-416E-B23F-1ED7CCF7A250}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A8C0414D-BED6-42D6-8DFF-34CF71ED14E0}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" srcOrd="2" destOrd="0" parTransId="{64A45BF4-F96D-4154-B896-A2968F8013A7}" sibTransId="{67E78DAB-94A4-4E9D-98CC-77C1C6804395}"/>
-    <dgm:cxn modelId="{A2CFE446-F7AF-4625-9038-66F953BC2E23}" type="presOf" srcId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" destId="{5D8738F3-1038-4DB7-90C8-BC0BCD90DD29}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{502D1E8E-ABC4-4B81-B07D-71307B16B28A}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{92B83617-ED82-479A-81AB-48E59441279A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{4852368D-7AEA-49C1-886B-CFF58430821B}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{E1F01CDD-5670-4739-9527-CEF58348CE13}" srcOrd="3" destOrd="0" parTransId="{61E3E20A-2669-484D-A61A-FACE97D57C50}" sibTransId="{7E81F9C3-E4FA-4D27-8D73-380C37F4FA1A}"/>
     <dgm:cxn modelId="{A73AD1F8-380E-4C75-A752-6AD7EAD4AF16}" srcId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" destId="{5AE34F33-E233-4260-8B3A-D2A952939B50}" srcOrd="0" destOrd="0" parTransId="{BBB0F776-4554-493F-B21B-A368FA081884}" sibTransId="{717A4BC5-2FD2-4D7A-912F-D3F9F37D4AC4}"/>
-    <dgm:cxn modelId="{ECA2396E-0B8D-4627-BE94-D3842C316098}" type="presOf" srcId="{92287CD8-E47A-42DE-84C3-A4BA177C1D62}" destId="{695642E2-B91F-4EE3-9EFF-1DFC56010147}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{30E66259-DDD1-4524-BB9A-CD51F25581B7}" type="presOf" srcId="{DED3A5A0-4712-42BF-9348-5C74F0E51A65}" destId="{9FA01DDC-66B0-409A-8BDE-2ACDFA7EA0A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9768AB10-23AB-47C4-874B-92CBB49B9235}" type="presOf" srcId="{A56A8A2E-51AC-4DDD-8C26-913299B6923C}" destId="{426E8D05-299B-4227-83F5-A25FDC0795CE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1E25BA0B-AA21-4599-8237-94C90FA1318F}" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" srcOrd="1" destOrd="0" parTransId="{9017723E-9271-414F-97DD-42C6B68B95A5}" sibTransId="{F3B1A03B-8586-468D-AB33-0AF66DB1B805}"/>
-    <dgm:cxn modelId="{E9B02B10-502A-4259-90D4-55EFAEE3D886}" type="presOf" srcId="{3DAA76D5-D6B2-4F1B-BA42-DBCDFC9BD7B6}" destId="{3D6067FF-2AC1-434B-8C23-95B06FAAB7DF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{258F77C6-606A-4A4C-AEC5-A513CB7AFD3F}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{7367E153-CE6E-45B1-8878-0762ECA2DD83}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{61575136-175D-4FEF-BE80-70AC48BEF140}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{308C6037-FADA-4F2B-8429-2A008A44D9F2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{33D79453-008A-4D1E-90E8-873B3083C39C}" srcId="{3635EF60-F64E-4EE3-B729-086102104583}" destId="{46FC912B-7276-4C81-9EBE-5E05C5ECF3CF}" srcOrd="0" destOrd="0" parTransId="{CD515B3C-8108-410F-9B6B-8E18B114EE86}" sibTransId="{5B17D466-83AB-4A1E-8366-95071FB481AC}"/>
-    <dgm:cxn modelId="{1C4FF281-C9D4-47E5-A2D9-21D4FA56AA3D}" type="presOf" srcId="{63808121-E830-4E2A-B990-90E7F621E30F}" destId="{D4124EAE-C9A4-44D7-8696-129097016723}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A96ED176-342B-4CCE-B6C9-05774EA877F2}" type="presOf" srcId="{4CAA0C04-4250-42A0-9D3F-24CA1E06880C}" destId="{5E40320B-C876-487B-B530-CDD6B4496081}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9031E8AF-6292-4901-914C-42E38AF62562}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{E74FDBBE-303A-48BD-9525-0327D908A1D2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{24736A80-AD67-4EE9-8F41-59367F394EF9}" type="presOf" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{9C6F0D09-7654-49E6-BEE9-F5798519A1C7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{79922E2F-2A52-48DE-9C7B-2E49DA66BAA6}" type="presOf" srcId="{9AD1FC72-C6DE-4496-8FC7-A54BAA2B6F67}" destId="{CDA58B6C-10C1-4268-A158-A858D216A50B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{98DBC49F-0FE8-49D1-A8E0-5BF18B6B56C6}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{019924A5-E93F-429E-913D-69BF8664489C}" srcOrd="0" destOrd="0" parTransId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" sibTransId="{B0E33302-3849-41D5-B325-A7A44C8028D5}"/>
-    <dgm:cxn modelId="{9B24C8EB-FEC3-4361-8F6A-C004F72B6CA5}" type="presOf" srcId="{C817EB3D-42B5-431C-AB56-2950092D941B}" destId="{CA7202EA-FC9B-469A-818E-C42165B0D395}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{24B53B70-2C73-4B1D-90C0-D891A86675A0}" type="presOf" srcId="{03ABD42A-0493-474B-B997-8FE86D8ED15E}" destId="{A7886049-F4A6-4B3E-BF2E-DBE90C832EAD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{2C948CFD-02CA-4B5C-B3F4-F0D8A68C91AE}" type="presOf" srcId="{04CB6FF8-7D74-42CA-B4C9-AC202554DD5B}" destId="{A2733577-E6F8-490F-BDFB-91F1859D51F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0027E26B-B643-4445-B18E-D376D30650B3}" srcId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" destId="{DE1A6187-7629-4A69-B770-B6DABFB03422}" srcOrd="2" destOrd="0" parTransId="{A2B04E9B-4E9E-44A6-8EC1-4EE8A9034AA0}" sibTransId="{BCE61832-DA7C-4F87-BB86-D5835E40DAB1}"/>
-    <dgm:cxn modelId="{EBD95D13-3837-406F-AF56-F1881EF797AA}" type="presOf" srcId="{50F256B0-FCD6-4530-B4AB-A2930578CC82}" destId="{144EFE5B-2652-4ADF-B7F7-8617B26DD151}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B008CD50-423B-4D30-8552-0611AF438E08}" type="presOf" srcId="{2E890CF8-8394-4470-B84E-E18D8932CFFC}" destId="{FECE3617-7B45-4E8D-A2CB-852EA32699A3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0FA33ECD-AB07-4C39-88F5-784DEA5392D4}" type="presOf" srcId="{EEA4340A-4629-4664-991A-F6D5767A0C87}" destId="{64252D07-EE7B-49E9-8905-77D83680C8CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{4AE052C3-7ADC-475C-B793-20DC671F3A9A}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{701B6EA1-42FC-4C72-A729-BFF0F219C36C}" srcOrd="1" destOrd="0" parTransId="{514D4F55-52C7-4443-B7BF-3E843E76B049}" sibTransId="{476294FA-2A8D-4342-AA14-A29092D8CBE3}"/>
-    <dgm:cxn modelId="{BDA0D26B-B83B-49E6-B768-2EA20803F58D}" srcId="{5AC9A733-0F85-4966-BD31-B61EEF72F244}" destId="{791A7A13-9E89-42CE-924B-CA6906FE03C8}" srcOrd="1" destOrd="0" parTransId="{6B0B8C7C-68C3-4F35-9055-2DA1D61C0A6E}" sibTransId="{C5BEA234-398E-4E73-A1DA-697FAA886784}"/>
-    <dgm:cxn modelId="{D4EF41BA-3402-4E9D-A60D-C999F57A0E84}" type="presOf" srcId="{AA2EBC20-6471-423B-943B-DB7F60016B80}" destId="{95EC4EE2-724C-474F-A9E1-B85274F03474}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9FBC12D3-EC0F-4FFE-B35C-B96A516268B3}" type="presOf" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{398568D2-83C7-4580-90B1-59B85FA66394}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{40DA832C-FAE3-4AC1-BFAF-6393F8A574E2}" type="presOf" srcId="{95C85A58-7D8B-4CE0-A849-1AAD804D43CA}" destId="{EA0793E8-65F4-4383-82A2-4170B37B05B1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9C2291B3-6308-483B-8E34-9D7E5B8D8FDB}" type="presOf" srcId="{3C9BA8C6-C0FC-4AC9-B9E3-D45C90975F46}" destId="{FB94CB6F-F13A-4A1C-BC5B-21260572171F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{F6471420-45D0-4883-AA73-794106838C93}" type="presOf" srcId="{D93B2254-B950-48F0-A2EC-F47FDAD3662E}" destId="{B4FB48FE-BE0C-42D7-AE54-FF62EFDAA971}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{17AD505C-44DB-4307-A72F-1B5B07721D5A}" srcId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" destId="{54476BD3-5D72-4211-8A5F-213D3719457A}" srcOrd="1" destOrd="0" parTransId="{44BC9E85-EA61-459E-91E5-FA35091328A9}" sibTransId="{37B6B00B-0731-4ED2-ABCA-2078374C26AB}"/>
-    <dgm:cxn modelId="{FA6F9ACA-BB6A-4731-9A4B-D5D23818E8D3}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{85897CFB-EF2B-44E0-A3DB-C056D754EABF}" srcOrd="5" destOrd="0" parTransId="{623569C3-553D-47FC-917D-DD7627C010D4}" sibTransId="{246DAF3F-2D1D-4A7A-A18D-7CC64A61220B}"/>
-    <dgm:cxn modelId="{FC50FAD2-3727-4FE2-87C4-B5ADDCB292B0}" srcId="{5E6058FC-8D44-4D24-B5A1-50930E819B91}" destId="{D2945899-9B95-4912-9F0D-B097D73A85E8}" srcOrd="4" destOrd="0" parTransId="{C258E371-6010-423A-B89E-97F39B6E2061}" sibTransId="{D11DF62A-C599-40F2-883D-4E7E458CF1F8}"/>
-    <dgm:cxn modelId="{550FC2DC-30EA-4F6B-88A7-14D4D62B6D08}" type="presOf" srcId="{7B5443A0-F41B-49B4-9F69-78FE95DD9FA8}" destId="{40DFF878-6852-49C1-B90F-9D5F087C41E0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E8B7A71D-511C-48F7-BE47-FAE4F15A1514}" type="presOf" srcId="{0D7D100F-92B5-45B5-9725-E3A708939227}" destId="{43450866-70F5-4361-BB5A-08446B43F641}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{EE06ED72-436B-4261-85D9-5B0C5C947861}" type="presOf" srcId="{928A2C59-6030-4968-BFFD-1E0F0DA17451}" destId="{1DF726E4-1965-4D1B-B481-C845850FBD91}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C8106DA2-C15B-4E1D-BE48-04DF11A0A4B4}" type="presOf" srcId="{9D2B2C1B-7443-4BF9-8379-45B2F824EA78}" destId="{F7C0520F-A4DD-4BA0-8CE1-746C13CB31D3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{48B1619E-E55E-4A50-9BC2-C3DF86363710}" type="presOf" srcId="{6DAF27D7-E0B1-4E8D-ACA7-B6D8DA9F4056}" destId="{D57AF638-81DE-43EB-84E2-A59C7AAADE15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{980F6E64-2D07-4ACB-AB41-88F91366616B}" type="presOf" srcId="{1579B706-E4B7-43A2-8060-CF67A71C1E59}" destId="{A1413320-E1DA-4727-8163-71C9FBE3DAA6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{A2A34727-EEDD-4F7A-B70A-FADD1FED13E9}" type="presParOf" srcId="{CA7202EA-FC9B-469A-818E-C42165B0D395}" destId="{83E344F5-8732-4AE4-B4CF-AA653D5BC4D1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{3F8D4B7B-4C1F-43E7-8217-64B98642208E}" type="presParOf" srcId="{83E344F5-8732-4AE4-B4CF-AA653D5BC4D1}" destId="{26D0847B-F0A1-4E26-8E2B-16FCF79D4617}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{5EFA0D23-DF22-4371-BCF6-EC7E58F4AD0E}" type="presParOf" srcId="{26D0847B-F0A1-4E26-8E2B-16FCF79D4617}" destId="{46BFD23D-3D26-4D33-AAD7-A4D969EB893A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -4618,8 +4616,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8562643" y="1446866"/>
-          <a:ext cx="722927" cy="250933"/>
+          <a:off x="7656107" y="1344427"/>
+          <a:ext cx="670504" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4633,13 +4631,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="125466"/>
+                <a:pt x="670504" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="250933"/>
+                <a:pt x="670504" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4678,8 +4676,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7704969" y="2295260"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="6860628" y="2131301"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4693,10 +4691,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4735,8 +4733,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7579503" y="2295260"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="6744259" y="2131301"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4747,13 +4745,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="125466" y="0"/>
+                <a:pt x="116368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4792,8 +4790,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="15843273" y="4840444"/>
-          <a:ext cx="116330" cy="549664"/>
+          <a:off x="14231061" y="4491921"/>
+          <a:ext cx="110827" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4804,13 +4802,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="110827" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="116330" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4849,8 +4844,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14875386" y="3992050"/>
-          <a:ext cx="1445855" cy="250933"/>
+          <a:off x="13511083" y="3705048"/>
+          <a:ext cx="1274114" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4864,13 +4859,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1445855" y="125466"/>
+                <a:pt x="1274114" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1445855" y="250933"/>
+                <a:pt x="1274114" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4909,8 +4904,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14829666" y="3992050"/>
-          <a:ext cx="91440" cy="250933"/>
+          <a:off x="13465363" y="3705048"/>
+          <a:ext cx="91440" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4924,7 +4919,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="250933"/>
+                <a:pt x="45720" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4963,8 +4958,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="13429530" y="3992050"/>
-          <a:ext cx="1445855" cy="250933"/>
+          <a:off x="12170073" y="3705048"/>
+          <a:ext cx="1341009" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4975,16 +4970,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1445855" y="0"/>
+                <a:pt x="1341009" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1445855" y="125466"/>
+                <a:pt x="1341009" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="250933"/>
+                <a:pt x="0" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5023,8 +5018,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7704969" y="2295260"/>
-          <a:ext cx="7170416" cy="1099328"/>
+          <a:off x="6860628" y="2131301"/>
+          <a:ext cx="6650455" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5038,13 +5033,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="7170416" y="973861"/>
+                <a:pt x="6650455" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="7170416" y="1099328"/>
+                <a:pt x="6650455" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5083,8 +5078,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11704971" y="3992050"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="10570570" y="3705048"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5095,13 +5090,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="125466" y="0"/>
+                <a:pt x="116368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5140,8 +5135,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="12427899" y="5688839"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="11241075" y="5278795"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5152,13 +5147,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="125466" y="0"/>
+                <a:pt x="116368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5197,8 +5192,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11830438" y="3992050"/>
-          <a:ext cx="722927" cy="1099328"/>
+          <a:off x="10686938" y="3705048"/>
+          <a:ext cx="670504" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5212,13 +5207,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="973861"/>
+                <a:pt x="670504" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="1099328"/>
+                <a:pt x="670504" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5257,8 +5252,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11107510" y="3992050"/>
-          <a:ext cx="722927" cy="1099328"/>
+          <a:off x="10016434" y="3705048"/>
+          <a:ext cx="670504" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5269,16 +5264,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="722927" y="0"/>
+                <a:pt x="670504" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="722927" y="973861"/>
+                <a:pt x="670504" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="1099328"/>
+                <a:pt x="0" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5317,8 +5312,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7704969" y="2295260"/>
-          <a:ext cx="4125468" cy="1099328"/>
+          <a:off x="6860628" y="2131301"/>
+          <a:ext cx="3826310" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5332,13 +5327,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="4125468" y="973861"/>
+                <a:pt x="3826310" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="4125468" y="1099328"/>
+                <a:pt x="3826310" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5377,8 +5372,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7492871" y="3992050"/>
-          <a:ext cx="2168783" cy="250933"/>
+          <a:off x="6663909" y="3705048"/>
+          <a:ext cx="2011514" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5392,13 +5387,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2168783" y="125466"/>
+                <a:pt x="2011514" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2168783" y="250933"/>
+                <a:pt x="2011514" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5437,8 +5432,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7737830" y="4840444"/>
-          <a:ext cx="179238" cy="715059"/>
+          <a:off x="6891105" y="4491921"/>
+          <a:ext cx="166240" cy="663206"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5452,10 +5447,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="715059"/>
+                <a:pt x="0" y="663206"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="715059"/>
+                <a:pt x="166240" y="663206"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5494,8 +5489,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7492871" y="3992050"/>
-          <a:ext cx="722927" cy="250933"/>
+          <a:off x="6663909" y="3705048"/>
+          <a:ext cx="670504" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5509,13 +5504,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="125466"/>
+                <a:pt x="670504" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="250933"/>
+                <a:pt x="670504" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5554,8 +5549,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6644476" y="4840444"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="5877036" y="4491921"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5566,13 +5561,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="125466" y="0"/>
+                <a:pt x="116368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5611,8 +5606,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6769943" y="3992050"/>
-          <a:ext cx="722927" cy="250933"/>
+          <a:off x="5993404" y="3705048"/>
+          <a:ext cx="670504" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5623,16 +5618,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="722927" y="0"/>
+                <a:pt x="670504" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="722927" y="125466"/>
+                <a:pt x="670504" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="250933"/>
+                <a:pt x="0" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5671,8 +5666,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5198620" y="4840444"/>
-          <a:ext cx="125466" cy="549664"/>
+          <a:off x="4536026" y="4491921"/>
+          <a:ext cx="116368" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5683,13 +5678,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="125466" y="0"/>
+                <a:pt x="116368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="125466" y="549664"/>
+                <a:pt x="116368" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5728,8 +5723,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5324087" y="3992050"/>
-          <a:ext cx="2168783" cy="250933"/>
+          <a:off x="4652395" y="3705048"/>
+          <a:ext cx="2011514" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5740,16 +5735,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="2168783" y="0"/>
+                <a:pt x="2011514" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="2168783" y="125466"/>
+                <a:pt x="2011514" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="250933"/>
+                <a:pt x="0" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5788,8 +5783,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7492871" y="2295260"/>
-          <a:ext cx="212098" cy="1099328"/>
+          <a:off x="6663909" y="2131301"/>
+          <a:ext cx="196718" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5800,16 +5795,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="212098" y="0"/>
+                <a:pt x="196718" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="212098" y="973861"/>
+                <a:pt x="196718" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="1099328"/>
+                <a:pt x="0" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5848,8 +5843,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2378604" y="3992050"/>
-          <a:ext cx="179238" cy="3094848"/>
+          <a:off x="1920503" y="3705048"/>
+          <a:ext cx="166240" cy="2870425"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5863,10 +5858,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="3094848"/>
+                <a:pt x="0" y="2870425"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="3094848"/>
+                <a:pt x="166240" y="2870425"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5905,8 +5900,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2378604" y="3992050"/>
-          <a:ext cx="179238" cy="2246453"/>
+          <a:off x="1920503" y="3705048"/>
+          <a:ext cx="166240" cy="2083552"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5920,10 +5915,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="2246453"/>
+                <a:pt x="0" y="2083552"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="2246453"/>
+                <a:pt x="166240" y="2083552"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5962,8 +5957,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2378604" y="3992050"/>
-          <a:ext cx="179238" cy="1398058"/>
+          <a:off x="1920503" y="3705048"/>
+          <a:ext cx="166240" cy="1296678"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5977,10 +5972,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="1398058"/>
+                <a:pt x="0" y="1296678"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="1398058"/>
+                <a:pt x="166240" y="1296678"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6019,8 +6014,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2378604" y="3992050"/>
-          <a:ext cx="179238" cy="549664"/>
+          <a:off x="1920503" y="3705048"/>
+          <a:ext cx="166240" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6034,10 +6029,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="549664"/>
+                <a:pt x="166240" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6076,8 +6071,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2856573" y="2295260"/>
-          <a:ext cx="4848396" cy="1099328"/>
+          <a:off x="2363812" y="2131301"/>
+          <a:ext cx="4496815" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6088,16 +6083,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="4848396" y="0"/>
+                <a:pt x="4496815" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="4848396" y="973861"/>
+                <a:pt x="4496815" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="1099328"/>
+                <a:pt x="0" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6136,8 +6131,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="932749" y="3992050"/>
-          <a:ext cx="179238" cy="1398058"/>
+          <a:off x="579493" y="3705048"/>
+          <a:ext cx="166240" cy="1296678"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6151,10 +6146,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="1398058"/>
+                <a:pt x="0" y="1296678"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="1398058"/>
+                <a:pt x="166240" y="1296678"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6193,8 +6188,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="932749" y="3992050"/>
-          <a:ext cx="179238" cy="549664"/>
+          <a:off x="579493" y="3705048"/>
+          <a:ext cx="166240" cy="509805"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6208,10 +6203,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="549664"/>
+                <a:pt x="0" y="509805"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="179238" y="549664"/>
+                <a:pt x="166240" y="509805"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6250,8 +6245,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1410718" y="2295260"/>
-          <a:ext cx="6294251" cy="1099328"/>
+          <a:off x="1022802" y="2131301"/>
+          <a:ext cx="5837825" cy="1019610"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6262,16 +6257,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="6294251" y="0"/>
+                <a:pt x="5837825" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="6294251" y="973861"/>
+                <a:pt x="5837825" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="973861"/>
+                <a:pt x="0" y="903242"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="1099328"/>
+                <a:pt x="0" y="1019610"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6310,8 +6305,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7704969" y="1446866"/>
-          <a:ext cx="857673" cy="250933"/>
+          <a:off x="6860628" y="1344427"/>
+          <a:ext cx="795479" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6322,16 +6317,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="857673" y="0"/>
+                <a:pt x="795479" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="857673" y="125466"/>
+                <a:pt x="795479" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="250933"/>
+                <a:pt x="0" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6370,8 +6365,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7839715" y="598471"/>
-          <a:ext cx="722927" cy="250933"/>
+          <a:off x="6985602" y="557554"/>
+          <a:ext cx="670504" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6385,13 +6380,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="125466"/>
+                <a:pt x="670504" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="722927" y="250933"/>
+                <a:pt x="670504" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6430,8 +6425,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7116787" y="598471"/>
-          <a:ext cx="722927" cy="250933"/>
+          <a:off x="6315097" y="557554"/>
+          <a:ext cx="670504" cy="232737"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6442,16 +6437,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="722927" y="0"/>
+                <a:pt x="670504" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="722927" y="125466"/>
+                <a:pt x="670504" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="125466"/>
+                <a:pt x="0" y="116368"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="250933"/>
+                <a:pt x="0" y="232737"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6490,8 +6485,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7242254" y="1010"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="6431466" y="3417"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6557,8 +6552,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7242254" y="1010"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="6431466" y="3417"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{03FB1A03-C635-4199-880D-D1975DFAC8B4}">
@@ -6568,8 +6563,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6519326" y="849405"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="5760961" y="790291"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6635,8 +6630,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6519326" y="849405"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="5760961" y="790291"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E74FDBBE-303A-48BD-9525-0327D908A1D2}">
@@ -6646,8 +6641,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7965182" y="849405"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="7101971" y="790291"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6713,8 +6708,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7965182" y="849405"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="7101971" y="790291"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B44048FB-FF46-4440-A04E-4D04E7A269DA}">
@@ -6724,8 +6719,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7107508" y="1697799"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="6306491" y="1577164"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6791,8 +6786,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7107508" y="1697799"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="6306491" y="1577164"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{173AA79E-2FF2-42D4-B70B-D125E9A80658}">
@@ -6802,8 +6797,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="813257" y="3394588"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="468666" y="3150911"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6869,8 +6864,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="813257" y="3394588"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="468666" y="3150911"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CBF4E0AE-D8D2-4311-82F7-B8881C50572D}">
@@ -6880,8 +6875,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1111987" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="745734" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6947,8 +6942,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1111987" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="745734" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{43450866-70F5-4361-BB5A-08446B43F641}">
@@ -6958,8 +6953,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1111987" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="745734" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7025,8 +7020,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1111987" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="745734" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{32ABA577-60BD-4197-902B-F86B9051CAE1}">
@@ -7036,8 +7031,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2259112" y="3394588"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="1809676" y="3150911"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7103,8 +7098,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2259112" y="3394588"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="1809676" y="3150911"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{64252D07-EE7B-49E9-8905-77D83680C8CF}">
@@ -7114,8 +7109,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2557843" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="2086744" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7181,8 +7176,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2557843" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="2086744" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B4FB48FE-BE0C-42D7-AE54-FF62EFDAA971}">
@@ -7192,8 +7187,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2557843" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="2086744" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7259,8 +7254,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2557843" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="2086744" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{FADF29D8-DCE3-42EC-868B-6E3678942948}">
@@ -7270,8 +7265,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2557843" y="5939772"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="2086744" y="5511532"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7337,8 +7332,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2557843" y="5939772"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="2086744" y="5511532"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A1413320-E1DA-4727-8163-71C9FBE3DAA6}">
@@ -7348,8 +7343,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2557843" y="6788167"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="2086744" y="6298405"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7415,8 +7410,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2557843" y="6788167"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="2086744" y="6298405"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{ADD10C73-D834-4826-9754-A662C8A7E1FC}">
@@ -7426,8 +7421,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6895410" y="3394588"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="6109773" y="3150911"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7493,8 +7488,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6895410" y="3394588"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="6109773" y="3150911"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F2F22B34-EF56-4B93-8AE8-5CF39DB57AEC}">
@@ -7504,8 +7499,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4726626" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="4098258" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7571,8 +7566,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4726626" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="4098258" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2CAE613B-01AD-404A-B46B-B5DC3F4158E2}">
@@ -7582,8 +7577,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4003698" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="3427754" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7649,8 +7644,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4003698" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="3427754" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B978A0BD-405C-4642-9A48-ACCBC26BAC87}">
@@ -7660,8 +7655,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6172482" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="5439268" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7727,8 +7722,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6172482" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="5439268" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7137C75B-9DFD-4BD4-820F-1EF47882DDDC}">
@@ -7738,8 +7733,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5449554" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="4768763" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7805,8 +7800,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5449554" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="4768763" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{D4124EAE-C9A4-44D7-8696-129097016723}">
@@ -7816,8 +7811,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7618338" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="6780278" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7883,8 +7878,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7618338" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="6780278" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E87EAE8A-6AEE-42F9-89D6-97AAC447F7F2}">
@@ -7894,8 +7889,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7917068" y="5091378"/>
-          <a:ext cx="1194922" cy="928251"/>
+          <a:off x="7057346" y="4724658"/>
+          <a:ext cx="1108272" cy="860939"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7961,8 +7956,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7917068" y="5091378"/>
-        <a:ext cx="1194922" cy="928251"/>
+        <a:off x="7057346" y="4724658"/>
+        <a:ext cx="1108272" cy="860939"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3D6067FF-2AC1-434B-8C23-95B06FAAB7DF}">
@@ -7972,8 +7967,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9064193" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="8121288" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8039,8 +8034,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="9064193" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="8121288" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{398568D2-83C7-4580-90B1-59B85FA66394}">
@@ -8050,8 +8045,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11232977" y="3394588"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="10132802" y="3150911"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8117,8 +8112,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11232977" y="3394588"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="10132802" y="3150911"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7367E153-CE6E-45B1-8878-0762ECA2DD83}">
@@ -8128,8 +8123,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10510049" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="9462297" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8195,8 +8190,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="10510049" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="9462297" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F2E83ED8-89A8-4994-8635-839B45715E66}">
@@ -8206,8 +8201,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11955905" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="10803307" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8273,8 +8268,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11955905" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="10803307" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{ACD37203-AD9C-4240-AEB3-595C59E85038}">
@@ -8284,8 +8279,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11232977" y="5939772"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="10132802" y="5511532"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8351,8 +8346,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11232977" y="5939772"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="10132802" y="5511532"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9362CB1F-15CC-4695-A870-B772FD72C8CC}">
@@ -8362,8 +8357,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10510049" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="9462297" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8429,8 +8424,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="10510049" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="9462297" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{26ED289C-3010-4451-ADDD-F478A5C75B6B}">
@@ -8440,8 +8435,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14277925" y="3394588"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="12956946" y="3150911"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8507,8 +8502,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="14277925" y="3394588"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="12956946" y="3150911"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{78A08CF4-A659-46B7-A9CC-0C0438B9EB76}">
@@ -8518,8 +8513,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="12832069" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="11615937" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8585,8 +8580,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="12832069" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="11615937" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{92B83617-ED82-479A-81AB-48E59441279A}">
@@ -8596,8 +8591,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14277925" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="12956946" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8663,8 +8658,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="14277925" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="12956946" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8686384B-DEFF-498F-B380-F68C33BD97BB}">
@@ -8674,8 +8669,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="15723781" y="4242983"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="14231061" y="3937785"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8741,8 +8736,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="15723781" y="4242983"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="14231061" y="3937785"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0FC862D5-A8A5-4AA8-9ED4-6BE56788C7B3}">
@@ -8752,8 +8747,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="15959603" y="5091378"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="14231061" y="4724658"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8819,8 +8814,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="15959603" y="5091378"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="14231061" y="4724658"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3B170B0A-5CFE-4B48-8852-4B9BABF27377}">
@@ -8830,8 +8825,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6384581" y="2546194"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="5635986" y="2364038"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8892,8 +8887,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6384581" y="2546194"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="5635986" y="2364038"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{65FE7A1F-0558-481B-B958-A369D0BC2A1D}">
@@ -8903,8 +8898,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7830436" y="2546194"/>
-          <a:ext cx="1194922" cy="597461"/>
+          <a:off x="6976996" y="2364038"/>
+          <a:ext cx="1108272" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8965,8 +8960,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7830436" y="2546194"/>
-        <a:ext cx="1194922" cy="597461"/>
+        <a:off x="6976996" y="2364038"/>
+        <a:ext cx="1108272" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{82458DB8-1422-4E5B-B162-76C0E86E009E}">
@@ -8976,8 +8971,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8553364" y="1697799"/>
-          <a:ext cx="1464412" cy="597461"/>
+          <a:off x="7647501" y="1577164"/>
+          <a:ext cx="1358221" cy="554136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9043,8 +9038,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8553364" y="1697799"/>
-        <a:ext cx="1464412" cy="597461"/>
+        <a:off x="7647501" y="1577164"/>
+        <a:ext cx="1358221" cy="554136"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -11555,11 +11550,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11574,13 +11569,13 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="29.25" thickBot="1">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -11592,7 +11587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -11600,7 +11595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -11612,7 +11607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -11620,7 +11615,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -11628,7 +11623,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -11636,7 +11631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15" thickBot="1">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -11646,7 +11641,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -11663,7 +11658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="16.5" thickBot="1">
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -11680,7 +11675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.75">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
@@ -11695,52 +11690,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B10:E14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="47.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>